<commit_message>
更新 main 專案 - 2025-12-26 00:23:30
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -7,16 +7,17 @@
     <workbookView windowWidth="21882" windowHeight="11057"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
+    <sheet name="攻擊" sheetId="2" r:id="rId2"/>
+    <sheet name="動畫設計" sheetId="3" r:id="rId3"/>
+    <sheet name="場景規劃" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
   <si>
     <t>Devlog</t>
   </si>
@@ -30,48 +31,413 @@
     <t>實現敵人技能槽安裝，於Enemy.Initailized()時，呼叫SkillComponent.EquipEnemySkill()進行初始技能安裝。</t>
   </si>
   <si>
+    <t>裝備為主(傷害提高主要來源)、技能等級為輔、技能等級達頂轉職</t>
+  </si>
+  <si>
     <t>實現攻擊渲染Sprite圖層修正</t>
   </si>
   <si>
-    <t>敵人血量顯示異常修正</t>
+    <t>主角大招、奧義(特寫子彈時間)強大特效，玩家選擇範圍</t>
   </si>
   <si>
     <t>腳色Animation修正Player01、Player02、Enemy01</t>
   </si>
   <si>
+    <t>玩家血量提高(增加怪物連擊的可能性)、敵人攻擊範圍隱藏、鼓勵體會被攻擊、死亡懲罰略提高</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enemy04動畫修正，02、03腳色整體修正</t>
+  </si>
+  <si>
+    <t>玩家不移動，戰士格黨、弓手閃避提高、法師(血少)集氣後無敵</t>
+  </si>
+  <si>
+    <t>嘗試將敵人開始移動與停止移動動畫事件設定</t>
+  </si>
+  <si>
+    <t>敵人行為樹：攻擊(帶後搖)-&gt;朝向移動-&gt;正常移動-&gt;待機</t>
+  </si>
+  <si>
+    <t>成功將敵人移動邏輯修正完畢!可以根據動畫有正確的速度關係!</t>
+  </si>
+  <si>
+    <t>敵人血量HpSlider修正</t>
+  </si>
+  <si>
+    <t>玩家及敵人攻擊面向修正
+移動攻擊動畫邏輯及動畫修正
+樹精技能實現</t>
+  </si>
+  <si>
     <t>小灰鳥技能實現</t>
   </si>
   <si>
-    <t xml:space="preserve"> Enemy04動畫修正，02、03腳色整體修正</t>
-  </si>
-  <si>
     <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現</t>
   </si>
   <si>
-    <t>嘗試將敵人開始移動與停止移動動畫事件設定</t>
-  </si>
-  <si>
-    <t>移動方式決策，玩家維持，敵人移動改由AnimationEvent觸發(並傳入動畫長短)，控制移動距離長短。</t>
-  </si>
-  <si>
-    <t>成功將敵人移動邏輯修正完畢!可以根據動畫有正確的速度關係!</t>
-  </si>
-  <si>
-    <t>樹精技能實現</t>
+    <t>攻擊要素</t>
+  </si>
+  <si>
+    <t>備註</t>
+  </si>
+  <si>
+    <t>時機</t>
+  </si>
+  <si>
+    <t>接近性</t>
+  </si>
+  <si>
+    <t>距離</t>
+  </si>
+  <si>
+    <t>併發性</t>
+  </si>
+  <si>
+    <t>最複雜多樣化的部分、大幅的影響遊戲體驗及遊戲平衡性，限制、控制敵方每秒傷害的總和</t>
+  </si>
+  <si>
+    <t>方向(攻擊、攝像機)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>一</t>
+  </si>
+  <si>
+    <t>對目標感知</t>
+  </si>
+  <si>
+    <t>攻擊方向</t>
+  </si>
+  <si>
+    <t>攻擊者分配</t>
+  </si>
+  <si>
+    <t>管理系統</t>
+  </si>
+  <si>
+    <t>選擇行動</t>
+  </si>
+  <si>
+    <t>根據狀態、規則、其他要素或隨機。</t>
+  </si>
+  <si>
+    <t>行動準備</t>
+  </si>
+  <si>
+    <t>預期框架</t>
+  </si>
+  <si>
+    <t>可識別行動</t>
+  </si>
+  <si>
+    <t>命中幀</t>
+  </si>
+  <si>
+    <t>攻擊間格幀</t>
+  </si>
+  <si>
+    <t>解析度幀</t>
+  </si>
+  <si>
+    <t>恢復平衡</t>
+  </si>
+  <si>
+    <t>恢復到待機</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>近戰攻擊</t>
+  </si>
+  <si>
+    <t>攻擊位移</t>
+  </si>
+  <si>
+    <t>遠距攻擊</t>
+  </si>
+  <si>
+    <t>範圍顯示、特效顯示</t>
+  </si>
+  <si>
+    <t>空間大小</t>
+  </si>
+  <si>
+    <t>小:距離近，大:距離遠</t>
+  </si>
+  <si>
+    <t>障礙物</t>
+  </si>
+  <si>
+    <t>掩體、窄道、大型障礙物</t>
+  </si>
+  <si>
+    <t>移動限制</t>
+  </si>
+  <si>
+    <t>地塊破壞、速度影響</t>
+  </si>
+  <si>
+    <t>陷阱物件</t>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>1V1決鬥V2甚至V3</t>
+  </si>
+  <si>
+    <t>Boss戰，截然不同的遊戲體驗，與普通敵人強大的對比</t>
+  </si>
+  <si>
+    <t>1V多</t>
+  </si>
+  <si>
+    <t>免費攻擊者遊戲</t>
+  </si>
+  <si>
+    <t>無高階系統控制、限制多敵人時的攻擊頻率</t>
+  </si>
+  <si>
+    <t>攻擊票</t>
+  </si>
+  <si>
+    <t>玩家戰鬥體驗變得可控、避免玩家不知所措。難度提高可提高敵人攻擊頻率</t>
+  </si>
+  <si>
+    <t>敵人來襲數量票</t>
+  </si>
+  <si>
+    <t>敵人種類區分</t>
+  </si>
+  <si>
+    <t>普通敵人(可預測)、高階敵人(複雜、挑戰性)有特別標示比如紅框、金框、籃框、綠框)</t>
+  </si>
+  <si>
+    <t>生存類</t>
+  </si>
+  <si>
+    <t>被敵人淹沒、不使用攻擊票、使用控制敵人生成數量</t>
+  </si>
+  <si>
+    <t>合作類</t>
+  </si>
+  <si>
+    <t>分散攻擊目標</t>
+  </si>
+  <si>
+    <t>混亂程度</t>
+  </si>
+  <si>
+    <t>小:更容易被解析</t>
+  </si>
+  <si>
+    <t>可控性</t>
+  </si>
+  <si>
+    <t>控制得越少，就越有即時感</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>視角</t>
+  </si>
+  <si>
+    <t>第一人稱、第三人稱、側視、俯視</t>
+  </si>
+  <si>
+    <t>俯視、側視</t>
+  </si>
+  <si>
+    <t>考慮同時顯示所有具威脅性敵人</t>
+  </si>
+  <si>
+    <t>螢幕外攻擊</t>
+  </si>
+  <si>
+    <t>預警提示(重要性有待評估)</t>
+  </si>
+  <si>
+    <t>攝影機風格</t>
+  </si>
+  <si>
+    <t>影響場景設計</t>
+  </si>
+  <si>
+    <t>受擊狀態</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>畏縮flinch</t>
+  </si>
+  <si>
+    <t>被打瞬間的小退縮、抖一下、不位移</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>踉蹌stumble</t>
+  </si>
+  <si>
+    <t>身體失衡、後退一步</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>硬直hitstun</t>
+  </si>
+  <si>
+    <t>不能動、不能出招</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>擊退knockback</t>
+  </si>
+  <si>
+    <t>被推飛一段距離</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>擊倒knockdown</t>
+  </si>
+  <si>
+    <t>倒地(較長時間)</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>浮空airborne</t>
+  </si>
+  <si>
+    <t>被打飛到空中</t>
+  </si>
+  <si>
+    <t>安排敵人位置</t>
+  </si>
+  <si>
+    <t>有利於訓練玩家控制能力</t>
+  </si>
+  <si>
+    <t>螢幕外的攻擊</t>
+  </si>
+  <si>
+    <t>讓玩家感覺並非無敵、降低掌控感</t>
+  </si>
+  <si>
+    <t>戰士大招</t>
+  </si>
+  <si>
+    <t>連續劈斬*5，大橫斬*1</t>
+  </si>
+  <si>
+    <t>遠景</t>
+  </si>
+  <si>
+    <t>顏色</t>
+  </si>
+  <si>
+    <t>飽和低、對比低</t>
+  </si>
+  <si>
+    <t>細節</t>
+  </si>
+  <si>
+    <t>幾乎沒線條感</t>
+  </si>
+  <si>
+    <t>大小</t>
+  </si>
+  <si>
+    <t>物件比中景大且模糊</t>
+  </si>
+  <si>
+    <t>中景</t>
+  </si>
+  <si>
+    <t>飽和中、別太亮、地面比角色暗一點</t>
+  </si>
+  <si>
+    <t>輪廓清楚</t>
+  </si>
+  <si>
+    <t>物件符合角色比例</t>
+  </si>
+  <si>
+    <t>前景</t>
+  </si>
+  <si>
+    <t>比中景更暗、偏同色系、透明度50-80</t>
+  </si>
+  <si>
+    <t>邊角、偶爾、別出現在腳色臉上</t>
+  </si>
+  <si>
+    <t>調色</t>
+  </si>
+  <si>
+    <t>主色系(80%物件同色系)</t>
+  </si>
+  <si>
+    <t>黃綠（溫暖、安全）</t>
+  </si>
+  <si>
+    <t>藍綠（神秘、深林）</t>
+  </si>
+  <si>
+    <t>冷灰綠（危險、敵多）</t>
+  </si>
+  <si>
+    <t>飽和度</t>
+  </si>
+  <si>
+    <t>玩家最高
+敵人高
+中景中
+前景中偏低
+遠景低</t>
+  </si>
+  <si>
+    <t>物件數量</t>
+  </si>
+  <si>
+    <t>大物件(樹木、瀑布1-2)
+中物件(橋、遺跡2-3)
+小物件(草、蘑菇)自由</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -107,7 +473,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,59 +511,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
@@ -182,7 +518,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="新細明體"/>
       <charset val="134"/>
@@ -192,36 +528,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,6 +548,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -249,8 +592,31 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,7 +625,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,31 +781,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,145 +817,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,35 +861,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -542,6 +891,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -556,176 +923,226 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1079,1363 +1496,1376 @@
   <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.9805825242718" style="2" customWidth="1"/>
-    <col min="2" max="2" width="72.2330097087379" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.766990291262" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="12.9805825242718" style="15" customWidth="1"/>
+    <col min="2" max="2" width="72.2330097087379" style="15" customWidth="1"/>
+    <col min="3" max="3" width="105.766990291262" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="18.45" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="14" customFormat="1" ht="18.45" spans="1:3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="36.85" spans="1:2">
-      <c r="A2" s="2">
+    <row r="2" ht="36.85" spans="1:3">
+      <c r="A2" s="15">
         <v>105</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" ht="18.45" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="15">
         <v>106</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="18.45" spans="1:3">
-      <c r="A4" s="2">
+      <c r="C3" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="36.85" spans="1:3">
+      <c r="A4" s="15">
         <v>107</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="17" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" ht="18.45" spans="1:3">
-      <c r="A5" s="2">
+      <c r="A5" s="15">
         <v>108</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="36.85" spans="1:3">
-      <c r="A6" s="2">
+      <c r="C5" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="18.45" spans="1:3">
+      <c r="A6" s="15">
         <v>109</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" ht="36.85" spans="1:3">
-      <c r="A7" s="2">
+      <c r="A7" s="15">
         <v>110</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2">
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" ht="18.45" spans="1:2">
+      <c r="A8" s="15">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="2">
+      <c r="B8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" ht="55.3" spans="1:3">
+      <c r="A9" s="15">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2">
+      <c r="B9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" ht="18.45" spans="1:3">
+      <c r="A10" s="15">
         <v>113</v>
       </c>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="2">
+      <c r="A11" s="15">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="2">
+      <c r="A12" s="15">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="2">
+      <c r="A13" s="15">
         <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="2">
+      <c r="A14" s="15">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="2">
+      <c r="A15" s="15">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="2">
+      <c r="A16" s="15">
         <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="2">
+      <c r="A17" s="15">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="2">
+      <c r="A18" s="15">
         <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="2">
+      <c r="A19" s="15">
         <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="2">
+      <c r="A20" s="15">
         <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="2">
+      <c r="A21" s="15">
         <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="2">
+      <c r="A22" s="15">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="2">
+      <c r="A23" s="15">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="2">
+      <c r="A24" s="15">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="2">
+      <c r="A25" s="15">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="2">
+      <c r="A26" s="15">
         <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="2">
+      <c r="A27" s="15">
         <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="2">
+      <c r="A28" s="15">
         <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="2">
+      <c r="A29" s="15">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="2">
+      <c r="A30" s="15">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="2">
+      <c r="A31" s="15">
         <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="2">
+      <c r="A32" s="15">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="2">
+      <c r="A33" s="15">
         <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="2">
+      <c r="A34" s="15">
         <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="2">
+      <c r="A35" s="15">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="2">
+      <c r="A36" s="15">
         <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="2">
+      <c r="A37" s="15">
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="2">
+      <c r="A38" s="15">
         <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="2">
+      <c r="A39" s="15">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="2">
+      <c r="A40" s="15">
         <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="2">
+      <c r="A41" s="15">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="2">
+      <c r="A42" s="15">
         <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="2">
+      <c r="A43" s="15">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="2">
+      <c r="A44" s="15">
         <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="2">
+      <c r="A45" s="15">
         <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="2">
+      <c r="A46" s="15">
         <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="2">
+      <c r="A47" s="15">
         <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="2">
+      <c r="A48" s="15">
         <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="2">
+      <c r="A49" s="15">
         <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="2">
+      <c r="A50" s="15">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="2">
+      <c r="A51" s="15">
         <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="2">
+      <c r="A52" s="15">
         <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="2">
+      <c r="A53" s="15">
         <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="2">
+      <c r="A54" s="15">
         <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="2">
+      <c r="A55" s="15">
         <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="2">
+      <c r="A56" s="15">
         <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="2">
+      <c r="A57" s="15">
         <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="2">
+      <c r="A58" s="15">
         <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="2">
+      <c r="A59" s="15">
         <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="2">
+      <c r="A60" s="15">
         <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="2">
+      <c r="A61" s="15">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="2">
+      <c r="A62" s="15">
         <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="2">
+      <c r="A63" s="15">
         <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="2">
+      <c r="A64" s="15">
         <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="2">
+      <c r="A65" s="15">
         <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="2">
+      <c r="A66" s="15">
         <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="2">
+      <c r="A67" s="15">
         <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="2">
+      <c r="A68" s="15">
         <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="2">
+      <c r="A69" s="15">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="2">
+      <c r="A70" s="15">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="2">
+      <c r="A71" s="15">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="2">
+      <c r="A72" s="15">
         <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="2">
+      <c r="A73" s="15">
         <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="2">
+      <c r="A74" s="15">
         <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="2">
+      <c r="A75" s="15">
         <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="2">
+      <c r="A76" s="15">
         <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="2">
+      <c r="A77" s="15">
         <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="2">
+      <c r="A78" s="15">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="2">
+      <c r="A79" s="15">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="2">
+      <c r="A80" s="15">
         <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="2">
+      <c r="A81" s="15">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="2">
+      <c r="A82" s="15">
         <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="2">
+      <c r="A83" s="15">
         <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="2">
+      <c r="A84" s="15">
         <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="2">
+      <c r="A85" s="15">
         <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="2">
+      <c r="A86" s="15">
         <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="2">
+      <c r="A87" s="15">
         <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="2">
+      <c r="A88" s="15">
         <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="2">
+      <c r="A89" s="15">
         <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="2">
+      <c r="A90" s="15">
         <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="2">
+      <c r="A91" s="15">
         <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="2">
+      <c r="A92" s="15">
         <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="2">
+      <c r="A93" s="15">
         <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="2">
+      <c r="A94" s="15">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="2">
+      <c r="A95" s="15">
         <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="2">
+      <c r="A96" s="15">
         <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="2">
+      <c r="A97" s="15">
         <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="2">
+      <c r="A98" s="15">
         <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="2">
+      <c r="A99" s="15">
         <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="2">
+      <c r="A100" s="15">
         <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="2">
+      <c r="A101" s="15">
         <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="2">
+      <c r="A102" s="15">
         <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="2">
+      <c r="A103" s="15">
         <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="2">
+      <c r="A104" s="15">
         <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="2">
+      <c r="A105" s="15">
         <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="2">
+      <c r="A106" s="15">
         <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="2">
+      <c r="A107" s="15">
         <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="2">
+      <c r="A108" s="15">
         <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="2">
+      <c r="A109" s="15">
         <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="2">
+      <c r="A110" s="15">
         <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="2">
+      <c r="A111" s="15">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="2">
+      <c r="A112" s="15">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="2">
+      <c r="A113" s="15">
         <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="2">
+      <c r="A114" s="15">
         <v>217</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="2">
+      <c r="A115" s="15">
         <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="2">
+      <c r="A116" s="15">
         <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="2">
+      <c r="A117" s="15">
         <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="2">
+      <c r="A118" s="15">
         <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="2">
+      <c r="A119" s="15">
         <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="2">
+      <c r="A120" s="15">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="2">
+      <c r="A121" s="15">
         <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="2">
+      <c r="A122" s="15">
         <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="2">
+      <c r="A123" s="15">
         <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="2">
+      <c r="A124" s="15">
         <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="2">
+      <c r="A125" s="15">
         <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="2">
+      <c r="A126" s="15">
         <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="2">
+      <c r="A127" s="15">
         <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="2">
+      <c r="A128" s="15">
         <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="2">
+      <c r="A129" s="15">
         <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="2">
+      <c r="A130" s="15">
         <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="2">
+      <c r="A131" s="15">
         <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="2">
+      <c r="A132" s="15">
         <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="2">
+      <c r="A133" s="15">
         <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="2">
+      <c r="A134" s="15">
         <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="2">
+      <c r="A135" s="15">
         <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="2">
+      <c r="A136" s="15">
         <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="2">
+      <c r="A137" s="15">
         <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="2">
+      <c r="A138" s="15">
         <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="2">
+      <c r="A139" s="15">
         <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="2">
+      <c r="A140" s="15">
         <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="2">
+      <c r="A141" s="15">
         <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="2">
+      <c r="A142" s="15">
         <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="2">
+      <c r="A143" s="15">
         <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="2">
+      <c r="A144" s="15">
         <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="2">
+      <c r="A145" s="15">
         <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="2">
+      <c r="A146" s="15">
         <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="2">
+      <c r="A147" s="15">
         <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="2">
+      <c r="A148" s="15">
         <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="2">
+      <c r="A149" s="15">
         <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="2">
+      <c r="A150" s="15">
         <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="2">
+      <c r="A151" s="15">
         <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="2">
+      <c r="A152" s="15">
         <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="2">
+      <c r="A153" s="15">
         <v>256</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="2">
+      <c r="A154" s="15">
         <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="2">
+      <c r="A155" s="15">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="2">
+      <c r="A156" s="15">
         <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="2">
+      <c r="A157" s="15">
         <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="2">
+      <c r="A158" s="15">
         <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="2">
+      <c r="A159" s="15">
         <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="2">
+      <c r="A160" s="15">
         <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="2">
+      <c r="A161" s="15">
         <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="2">
+      <c r="A162" s="15">
         <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="2">
+      <c r="A163" s="15">
         <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="2">
+      <c r="A164" s="15">
         <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="2">
+      <c r="A165" s="15">
         <v>268</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="2">
+      <c r="A166" s="15">
         <v>269</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="2">
+      <c r="A167" s="15">
         <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="2">
+      <c r="A168" s="15">
         <v>271</v>
       </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="2">
+      <c r="A169" s="15">
         <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="2">
+      <c r="A170" s="15">
         <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="2">
+      <c r="A171" s="15">
         <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="2">
+      <c r="A172" s="15">
         <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="2">
+      <c r="A173" s="15">
         <v>276</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="2">
+      <c r="A174" s="15">
         <v>277</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="2">
+      <c r="A175" s="15">
         <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="2">
+      <c r="A176" s="15">
         <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="2">
+      <c r="A177" s="15">
         <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="2">
+      <c r="A178" s="15">
         <v>281</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="2">
+      <c r="A179" s="15">
         <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="2">
+      <c r="A180" s="15">
         <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="2">
+      <c r="A181" s="15">
         <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="2">
+      <c r="A182" s="15">
         <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="2">
+      <c r="A183" s="15">
         <v>286</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="2">
+      <c r="A184" s="15">
         <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="2">
+      <c r="A185" s="15">
         <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="2">
+      <c r="A186" s="15">
         <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="2">
+      <c r="A187" s="15">
         <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="2">
+      <c r="A188" s="15">
         <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="2">
+      <c r="A189" s="15">
         <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="2">
+      <c r="A190" s="15">
         <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="2">
+      <c r="A191" s="15">
         <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="2">
+      <c r="A192" s="15">
         <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="2">
+      <c r="A193" s="15">
         <v>296</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="2">
+      <c r="A194" s="15">
         <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="2">
+      <c r="A195" s="15">
         <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="2">
+      <c r="A196" s="15">
         <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="2">
+      <c r="A197" s="15">
         <v>300</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="2">
+      <c r="A198" s="15">
         <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="2">
+      <c r="A199" s="15">
         <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="2">
+      <c r="A200" s="15">
         <v>303</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="2">
+      <c r="A201" s="15">
         <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="2">
+      <c r="A202" s="15">
         <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="2">
+      <c r="A203" s="15">
         <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="2">
+      <c r="A204" s="15">
         <v>307</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="2">
+      <c r="A205" s="15">
         <v>308</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="2">
+      <c r="A206" s="15">
         <v>309</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="2">
+      <c r="A207" s="15">
         <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="2">
+      <c r="A208" s="15">
         <v>311</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="2">
+      <c r="A209" s="15">
         <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="2">
+      <c r="A210" s="15">
         <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="2">
+      <c r="A211" s="15">
         <v>314</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="2">
+      <c r="A212" s="15">
         <v>315</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="2">
+      <c r="A213" s="15">
         <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="2">
+      <c r="A214" s="15">
         <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="2">
+      <c r="A215" s="15">
         <v>318</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="2">
+      <c r="A216" s="15">
         <v>319</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="2">
+      <c r="A217" s="15">
         <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="2">
+      <c r="A218" s="15">
         <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" s="2">
+      <c r="A219" s="15">
         <v>322</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="2">
+      <c r="A220" s="15">
         <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" s="2">
+      <c r="A221" s="15">
         <v>324</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="2">
+      <c r="A222" s="15">
         <v>325</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" s="2">
+      <c r="A223" s="15">
         <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="2">
+      <c r="A224" s="15">
         <v>327</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="2">
+      <c r="A225" s="15">
         <v>328</v>
       </c>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="2">
+      <c r="A226" s="15">
         <v>329</v>
       </c>
     </row>
     <row r="227" spans="1:1">
-      <c r="A227" s="2">
+      <c r="A227" s="15">
         <v>330</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="2">
+      <c r="A228" s="15">
         <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="2">
+      <c r="A229" s="15">
         <v>332</v>
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="2">
+      <c r="A230" s="15">
         <v>333</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="2">
+      <c r="A231" s="15">
         <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="2">
+      <c r="A232" s="15">
         <v>335</v>
       </c>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="2">
+      <c r="A233" s="15">
         <v>336</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="2">
+      <c r="A234" s="15">
         <v>337</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="2">
+      <c r="A235" s="15">
         <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="2">
+      <c r="A236" s="15">
         <v>339</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237" s="2">
+      <c r="A237" s="15">
         <v>340</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="2">
+      <c r="A238" s="15">
         <v>341</v>
       </c>
     </row>
     <row r="239" spans="1:1">
-      <c r="A239" s="2">
+      <c r="A239" s="15">
         <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="2">
+      <c r="A240" s="15">
         <v>343</v>
       </c>
     </row>
     <row r="241" spans="1:1">
-      <c r="A241" s="2">
+      <c r="A241" s="15">
         <v>344</v>
       </c>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="2">
+      <c r="A242" s="15">
         <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:1">
-      <c r="A243" s="2">
+      <c r="A243" s="15">
         <v>346</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="2">
+      <c r="A244" s="15">
         <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245" s="2">
+      <c r="A245" s="15">
         <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="2">
+      <c r="A246" s="15">
         <v>349</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" s="2">
+      <c r="A247" s="15">
         <v>350</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="2">
+      <c r="A248" s="15">
         <v>351</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" s="2">
+      <c r="A249" s="15">
         <v>352</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="2">
+      <c r="A250" s="15">
         <v>353</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" s="2">
+      <c r="A251" s="15">
         <v>354</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="2">
+      <c r="A252" s="15">
         <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:1">
-      <c r="A253" s="2">
+      <c r="A253" s="15">
         <v>356</v>
       </c>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="2">
+      <c r="A254" s="15">
         <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:1">
-      <c r="A255" s="2">
+      <c r="A255" s="15">
         <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="2">
+      <c r="A256" s="15">
         <v>359</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" s="2">
+      <c r="A257" s="15">
         <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="2">
+      <c r="A258" s="15">
         <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:1">
-      <c r="A259" s="2">
+      <c r="A259" s="15">
         <v>362</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="2">
+      <c r="A260" s="15">
         <v>363</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261" s="2">
+      <c r="A261" s="15">
         <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="2">
+      <c r="A262" s="15">
         <v>365</v>
       </c>
     </row>
@@ -2449,14 +2879,516 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="7.24271844660194" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.9708737864078" customWidth="1"/>
+    <col min="3" max="3" width="101.106796116505" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="7" customFormat="1" spans="1:3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:3">
+      <c r="A6" s="2"/>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="1" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A9" s="10">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" s="8" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A10" s="10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" s="8" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A11" s="10">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A12" s="10">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" s="8" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A13" s="10">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A14" s="10">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A15" s="10">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" s="8" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A16" s="10">
+        <v>9</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" s="8" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A17" s="10">
+        <v>10</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" s="7" customFormat="1" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" s="7" customFormat="1" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" s="7" customFormat="1" spans="1:3">
+      <c r="A39" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -2466,16 +3398,199 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10.3883495145631" customWidth="1"/>
+    <col min="2" max="2" width="31.7864077669903" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="8.66019417475728" style="2"/>
+    <col min="2" max="2" width="33.2912621359223" style="3" customWidth="1"/>
+    <col min="3" max="3" width="78.1359223300971" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.66019417475728" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" ht="77.15" spans="2:3">
+      <c r="B20" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" ht="46.3" spans="2:3">
+      <c r="B21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
更新 main 專案 - 2025-12-27 01:03:34
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21882" windowHeight="11057"/>
+    <workbookView windowWidth="28740" windowHeight="13542"/>
   </bookViews>
   <sheets>
     <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
     <sheet name="攻擊" sheetId="2" r:id="rId2"/>
     <sheet name="動畫設計" sheetId="3" r:id="rId3"/>
     <sheet name="場景規劃" sheetId="4" r:id="rId4"/>
+    <sheet name="概念設計" sheetId="5" r:id="rId5"/>
+    <sheet name="設計關鍵字" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248">
   <si>
     <t>Devlog</t>
   </si>
@@ -69,10 +71,27 @@
 樹精技能實現</t>
   </si>
   <si>
-    <t>小灰鳥技能實現</t>
+    <t>小灰鳥技能位移</t>
+  </si>
+  <si>
+    <t>開始按鈕太早按失效修復
+生成半徑太大偵測圓卡噸修復
+小灰鳥技能碰撞體實現</t>
   </si>
   <si>
     <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現</t>
+  </si>
+  <si>
+    <t>關卡通關、關卡失敗條件設定</t>
+  </si>
+  <si>
+    <t>腳色死亡動畫重製</t>
+  </si>
+  <si>
+    <t>腳色受傷動畫繪製</t>
+  </si>
+  <si>
+    <t>實際釋放技能後行為SkillDashType、SkillRecoveryType、DashSpeed、DashDuration、技能動畫分三段(中段持續循環)</t>
   </si>
   <si>
     <t>攻擊要素</t>
@@ -415,6 +434,356 @@
     <t>大物件(樹木、瀑布1-2)
 中物件(橋、遺跡2-3)
 小物件(草、蘑菇)自由</t>
+  </si>
+  <si>
+    <t>訓練法一：世界拆解練習（每天 15–30 分）</t>
+  </si>
+  <si>
+    <t>選一張你喜歡的概念圖，問這 5 題（寫下來）：</t>
+  </si>
+  <si>
+    <t>這是什麼世界？</t>
+  </si>
+  <si>
+    <t>誰住在這？</t>
+  </si>
+  <si>
+    <t>技術 / 時代？</t>
+  </si>
+  <si>
+    <t>氣候與資源？</t>
+  </si>
+  <si>
+    <t>如果做成遊戲，玩法是什麼？</t>
+  </si>
+  <si>
+    <t>訓練法二：限制式創作（最重要）</t>
+  </si>
+  <si>
+    <t>例如：</t>
+  </si>
+  <si>
+    <t>「只能用 3 種材質設計一個森林遺跡」</t>
+  </si>
+  <si>
+    <t>「沒有金屬的文明」</t>
+  </si>
+  <si>
+    <t>「長年暴雨的世界」</t>
+  </si>
+  <si>
+    <t>限制 = 設計誕生的地方</t>
+  </si>
+  <si>
+    <t>訓練法三：灰階世界（不要一開始上色）</t>
+  </si>
+  <si>
+    <t>先用明暗講清楚結構</t>
+  </si>
+  <si>
+    <t>再決定色彩情緒</t>
+  </si>
+  <si>
+    <t>最後才是細節</t>
+  </si>
+  <si>
+    <t>色彩是情緒，不是裝飾</t>
+  </si>
+  <si>
+    <t>訓練法四：世界模組化（非常適合你）</t>
+  </si>
+  <si>
+    <t>你可以這樣做（超適合獨立遊戲）：</t>
+  </si>
+  <si>
+    <t>樹木模組（3 種）</t>
+  </si>
+  <si>
+    <t>地形模組（斜坡 / 平地）</t>
+  </si>
+  <si>
+    <t>遺跡模組（牆 / 柱 / 門）</t>
+  </si>
+  <si>
+    <t>先定「規則」，再畫素材。</t>
+  </si>
+  <si>
+    <t>基本功(重要!所有的速成都是有代價的)</t>
+  </si>
+  <si>
+    <t>透視訓練</t>
+  </si>
+  <si>
+    <t>基本功，遠近變化!</t>
+  </si>
+  <si>
+    <r>
+      <t>收集、提煉參考參考</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1D41D5"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(概念設計的真正內功)</t>
+    </r>
+  </si>
+  <si>
+    <t>長年查閱參考資料、提煉參考資料的結果</t>
+  </si>
+  <si>
+    <t>手繪訓練</t>
+  </si>
+  <si>
+    <t>基礎語言與表達能力</t>
+  </si>
+  <si>
+    <t>基礎概念設計訓練</t>
+  </si>
+  <si>
+    <t>大量專業的知識儲備</t>
+  </si>
+  <si>
+    <t>分類不適想更多，而是「敢刪除」，選3-5個分類點，明確「不選什麼」</t>
+  </si>
+  <si>
+    <t>🕰 時間狀態</t>
+  </si>
+  <si>
+    <t>古代 / 現代/文明</t>
+  </si>
+  <si>
+    <t>殘破 / 完整</t>
+  </si>
+  <si>
+    <t>被遺棄 / 正在使用</t>
+  </si>
+  <si>
+    <t>🔺 形狀語言</t>
+  </si>
+  <si>
+    <t>圓形（自然、柔和、生命）</t>
+  </si>
+  <si>
+    <t>方形（人工、秩序、文明）</t>
+  </si>
+  <si>
+    <t>🎭 情緒調性</t>
+  </si>
+  <si>
+    <t>平靜 / 危險</t>
+  </si>
+  <si>
+    <t>神聖 / 詭異/邪惡</t>
+  </si>
+  <si>
+    <t>溫暖 / 冷清</t>
+  </si>
+  <si>
+    <t>角色</t>
+  </si>
+  <si>
+    <t>身分定位</t>
+  </si>
+  <si>
+    <t>自然之子/文明產物/混合</t>
+  </si>
+  <si>
+    <t>遺民/平民/流浪者/貴族</t>
+  </si>
+  <si>
+    <t>倖存者/守護者/探索者/逃亡者</t>
+  </si>
+  <si>
+    <t>生存狀態</t>
+  </si>
+  <si>
+    <t>健康/虛弱/受詛咒</t>
+  </si>
+  <si>
+    <t>成長中/停滯/衰敗</t>
+  </si>
+  <si>
+    <t>穩定/免強維生</t>
+  </si>
+  <si>
+    <t>圓潤/銳利</t>
+  </si>
+  <si>
+    <t>對稱/非對稱</t>
+  </si>
+  <si>
+    <t>簡潔/層層堆疊</t>
+  </si>
+  <si>
+    <t>材質與裝備來源</t>
+  </si>
+  <si>
+    <t>植物/皮革/石頭/金屬/玉器</t>
+  </si>
+  <si>
+    <t>自製/拾荒/傳承</t>
+  </si>
+  <si>
+    <t>修補痕跡/完整無損</t>
+  </si>
+  <si>
+    <t>儀式用/實戰</t>
+  </si>
+  <si>
+    <t>使用多久</t>
+  </si>
+  <si>
+    <t>誰負擔的起</t>
+  </si>
+  <si>
+    <t>量產/唯一</t>
+  </si>
+  <si>
+    <t>情緒氣質</t>
+  </si>
+  <si>
+    <t>溫和/冷靜/狂躁</t>
+  </si>
+  <si>
+    <t>孤獨/希望/麻木</t>
+  </si>
+  <si>
+    <t>神聖/世俗/異質</t>
+  </si>
+  <si>
+    <t>敵人</t>
+  </si>
+  <si>
+    <t>起源</t>
+  </si>
+  <si>
+    <t>自然誕生/人造失控/動植物/無機物</t>
+  </si>
+  <si>
+    <t>被污染 / 詛咒</t>
+  </si>
+  <si>
+    <t>古代殘留物</t>
+  </si>
+  <si>
+    <t>行為模式</t>
+  </si>
+  <si>
+    <t>巡邏/守護/獵食/侵蝕擴散</t>
+  </si>
+  <si>
+    <t>智慧層級</t>
+  </si>
+  <si>
+    <t>本能/簡單判斷/高度策略/模仿人類</t>
+  </si>
+  <si>
+    <t>威脅表現</t>
+  </si>
+  <si>
+    <t>體型壓迫/速度/數量/不可預測</t>
+  </si>
+  <si>
+    <t>裝備</t>
+  </si>
+  <si>
+    <t>用途</t>
+  </si>
+  <si>
+    <t>戰鬥/儀式/工具</t>
+  </si>
+  <si>
+    <t>日常/特殊情境</t>
+  </si>
+  <si>
+    <t>防禦/控制/爆發</t>
+  </si>
+  <si>
+    <t>製作文明</t>
+  </si>
+  <si>
+    <t>原始/古代高度文明/現代仿造/拼湊再利用</t>
+  </si>
+  <si>
+    <t>使用痕跡</t>
+  </si>
+  <si>
+    <t>全新/明顯磨損/修補過/破損仍可用</t>
+  </si>
+  <si>
+    <t>操作方式</t>
+  </si>
+  <si>
+    <t>粗暴/精準/需要技巧/需要條件</t>
+  </si>
+  <si>
+    <t>象徵性</t>
+  </si>
+  <si>
+    <t>物品</t>
+  </si>
+  <si>
+    <t>功能性</t>
+  </si>
+  <si>
+    <t>純功能/劇情觸發/世界觀說明/情緒裝飾</t>
+  </si>
+  <si>
+    <t>稀有度</t>
+  </si>
+  <si>
+    <t>常見/地區限定/世界唯一/已失傳</t>
+  </si>
+  <si>
+    <t>顏色區分(白/綠/藍/紫/黃/紅/黑)</t>
+  </si>
+  <si>
+    <t>所屬族群</t>
+  </si>
+  <si>
+    <t>平民/特定職業/古代文明/非人類</t>
+  </si>
+  <si>
+    <t>保存狀態</t>
+  </si>
+  <si>
+    <t>完好/半毀/被自然侵蝕/臨時拼湊</t>
+  </si>
+  <si>
+    <t>可讀性</t>
+  </si>
+  <si>
+    <t>一看就懂/需要解讀/誤導性外觀</t>
+  </si>
+  <si>
+    <t>場景</t>
+  </si>
+  <si>
+    <t>空間層級</t>
+  </si>
+  <si>
+    <t>前景(遮擋/氛圍)、中景(互動、戰鬥)、遠景(世界尺度)</t>
+  </si>
+  <si>
+    <t>主導力量</t>
+  </si>
+  <si>
+    <t>自然主導/人造主導/自然侵蝕文明/文明壓制自然</t>
+  </si>
+  <si>
+    <t>時間感</t>
+  </si>
+  <si>
+    <t>正在使用/剛被遺棄/荒廢已久/有節奏地重複</t>
+  </si>
+  <si>
+    <t>情緒目的</t>
+  </si>
+  <si>
+    <t>安全區/壓迫區/神秘區/過度區</t>
   </si>
 </sst>
 </file>
@@ -422,16 +791,32 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1D41D5"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -465,6 +850,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -472,15 +873,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,9 +921,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,7 +951,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -519,22 +959,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,86 +994,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -643,7 +1022,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,31 +1112,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,19 +1124,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,61 +1190,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,49 +1202,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,6 +1240,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -876,35 +1264,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -926,11 +1292,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -942,153 +1321,189 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1097,52 +1512,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1496,1376 +1899,1398 @@
   <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.9805825242718" style="15" customWidth="1"/>
-    <col min="2" max="2" width="72.2330097087379" style="15" customWidth="1"/>
-    <col min="3" max="3" width="105.766990291262" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="15"/>
+    <col min="1" max="1" width="12.9805825242718" style="23" customWidth="1"/>
+    <col min="2" max="2" width="72.2330097087379" style="23" customWidth="1"/>
+    <col min="3" max="3" width="105.766990291262" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="1" ht="18.45" spans="1:3">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="22" customFormat="1" ht="18.45" spans="1:3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="36.85" spans="1:3">
-      <c r="A2" s="15">
+      <c r="A2" s="23">
         <v>105</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="18.45" spans="1:3">
-      <c r="A3" s="15">
+      <c r="A3" s="23">
         <v>106</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="36.85" spans="1:3">
-      <c r="A4" s="15">
+      <c r="A4" s="23">
         <v>107</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="18.45" spans="1:3">
-      <c r="A5" s="15">
+      <c r="A5" s="23">
         <v>108</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="18.45" spans="1:3">
-      <c r="A6" s="15">
+      <c r="A6" s="23">
         <v>109</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" ht="36.85" spans="1:3">
-      <c r="A7" s="15">
+      <c r="A7" s="23">
         <v>110</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" ht="18.45" spans="1:2">
-      <c r="A8" s="15">
+      <c r="A8" s="23">
         <v>111</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="55.3" spans="1:3">
-      <c r="A9" s="15">
+      <c r="A9" s="23">
         <v>112</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="18.45" spans="1:3">
-      <c r="A10" s="15">
+    <row r="10" ht="55.3" spans="1:3">
+      <c r="A10" s="23">
         <v>113</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="15">
+      <c r="C10" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" ht="18.45" spans="1:3">
+      <c r="A11" s="23">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="15">
+      <c r="C11" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" ht="18.45" spans="1:3">
+      <c r="A12" s="23">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="15">
+      <c r="C12" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" ht="18.45" spans="1:3">
+      <c r="A13" s="23">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="15">
+      <c r="C13" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" ht="36.85" spans="1:3">
+      <c r="A14" s="23">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="15">
+      <c r="C14" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="23">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="15">
+      <c r="C15" s="27"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="23">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="15">
+      <c r="C16" s="27"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="23">
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="15">
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="23">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="15">
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="23">
         <v>122</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="15">
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="15">
+      <c r="C20" s="27"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23">
         <v>124</v>
       </c>
+      <c r="C21" s="27"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="15">
+      <c r="A22" s="23">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="15">
+      <c r="A23" s="23">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="15">
+      <c r="A24" s="23">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="15">
+      <c r="A25" s="23">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="15">
+      <c r="A26" s="23">
         <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="15">
+      <c r="A27" s="23">
         <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="15">
+      <c r="A28" s="23">
         <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="15">
+      <c r="A29" s="23">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="15">
+      <c r="A30" s="23">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="15">
+      <c r="A31" s="23">
         <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="15">
+      <c r="A32" s="23">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="15">
+      <c r="A33" s="23">
         <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="15">
+      <c r="A34" s="23">
         <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="15">
+      <c r="A35" s="23">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="15">
+      <c r="A36" s="23">
         <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="15">
+      <c r="A37" s="23">
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="15">
+      <c r="A38" s="23">
         <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="15">
+      <c r="A39" s="23">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="15">
+      <c r="A40" s="23">
         <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="15">
+      <c r="A41" s="23">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="15">
+      <c r="A42" s="23">
         <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="15">
+      <c r="A43" s="23">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="15">
+      <c r="A44" s="23">
         <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="15">
+      <c r="A45" s="23">
         <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="15">
+      <c r="A46" s="23">
         <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="15">
+      <c r="A47" s="23">
         <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="15">
+      <c r="A48" s="23">
         <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="15">
+      <c r="A49" s="23">
         <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="15">
+      <c r="A50" s="23">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="15">
+      <c r="A51" s="23">
         <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="15">
+      <c r="A52" s="23">
         <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="15">
+      <c r="A53" s="23">
         <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="15">
+      <c r="A54" s="23">
         <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="15">
+      <c r="A55" s="23">
         <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="15">
+      <c r="A56" s="23">
         <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="15">
+      <c r="A57" s="23">
         <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="15">
+      <c r="A58" s="23">
         <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="15">
+      <c r="A59" s="23">
         <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="15">
+      <c r="A60" s="23">
         <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="15">
+      <c r="A61" s="23">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="15">
+      <c r="A62" s="23">
         <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="15">
+      <c r="A63" s="23">
         <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="15">
+      <c r="A64" s="23">
         <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="15">
+      <c r="A65" s="23">
         <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="15">
+      <c r="A66" s="23">
         <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="15">
+      <c r="A67" s="23">
         <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="15">
+      <c r="A68" s="23">
         <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="15">
+      <c r="A69" s="23">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="15">
+      <c r="A70" s="23">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="15">
+      <c r="A71" s="23">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="15">
+      <c r="A72" s="23">
         <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="15">
+      <c r="A73" s="23">
         <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="15">
+      <c r="A74" s="23">
         <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="15">
+      <c r="A75" s="23">
         <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="15">
+      <c r="A76" s="23">
         <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="15">
+      <c r="A77" s="23">
         <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="15">
+      <c r="A78" s="23">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="15">
+      <c r="A79" s="23">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="15">
+      <c r="A80" s="23">
         <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="15">
+      <c r="A81" s="23">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="15">
+      <c r="A82" s="23">
         <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="15">
+      <c r="A83" s="23">
         <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="15">
+      <c r="A84" s="23">
         <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="15">
+      <c r="A85" s="23">
         <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="15">
+      <c r="A86" s="23">
         <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="15">
+      <c r="A87" s="23">
         <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="15">
+      <c r="A88" s="23">
         <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="15">
+      <c r="A89" s="23">
         <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="15">
+      <c r="A90" s="23">
         <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="15">
+      <c r="A91" s="23">
         <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="15">
+      <c r="A92" s="23">
         <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="15">
+      <c r="A93" s="23">
         <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="15">
+      <c r="A94" s="23">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="15">
+      <c r="A95" s="23">
         <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="15">
+      <c r="A96" s="23">
         <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="15">
+      <c r="A97" s="23">
         <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="15">
+      <c r="A98" s="23">
         <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="15">
+      <c r="A99" s="23">
         <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="15">
+      <c r="A100" s="23">
         <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="15">
+      <c r="A101" s="23">
         <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="15">
+      <c r="A102" s="23">
         <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="15">
+      <c r="A103" s="23">
         <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="15">
+      <c r="A104" s="23">
         <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="15">
+      <c r="A105" s="23">
         <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="15">
+      <c r="A106" s="23">
         <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="15">
+      <c r="A107" s="23">
         <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="15">
+      <c r="A108" s="23">
         <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="15">
+      <c r="A109" s="23">
         <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="15">
+      <c r="A110" s="23">
         <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="15">
+      <c r="A111" s="23">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="15">
+      <c r="A112" s="23">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="15">
+      <c r="A113" s="23">
         <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="15">
+      <c r="A114" s="23">
         <v>217</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="15">
+      <c r="A115" s="23">
         <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="15">
+      <c r="A116" s="23">
         <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="15">
+      <c r="A117" s="23">
         <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="15">
+      <c r="A118" s="23">
         <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="15">
+      <c r="A119" s="23">
         <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="15">
+      <c r="A120" s="23">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="15">
+      <c r="A121" s="23">
         <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="15">
+      <c r="A122" s="23">
         <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="15">
+      <c r="A123" s="23">
         <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="15">
+      <c r="A124" s="23">
         <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="15">
+      <c r="A125" s="23">
         <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="15">
+      <c r="A126" s="23">
         <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="15">
+      <c r="A127" s="23">
         <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="15">
+      <c r="A128" s="23">
         <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="15">
+      <c r="A129" s="23">
         <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="15">
+      <c r="A130" s="23">
         <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="15">
+      <c r="A131" s="23">
         <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="15">
+      <c r="A132" s="23">
         <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="15">
+      <c r="A133" s="23">
         <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="15">
+      <c r="A134" s="23">
         <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="15">
+      <c r="A135" s="23">
         <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="15">
+      <c r="A136" s="23">
         <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="15">
+      <c r="A137" s="23">
         <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="15">
+      <c r="A138" s="23">
         <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="15">
+      <c r="A139" s="23">
         <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="15">
+      <c r="A140" s="23">
         <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="15">
+      <c r="A141" s="23">
         <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="15">
+      <c r="A142" s="23">
         <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="15">
+      <c r="A143" s="23">
         <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="15">
+      <c r="A144" s="23">
         <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="15">
+      <c r="A145" s="23">
         <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="15">
+      <c r="A146" s="23">
         <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="15">
+      <c r="A147" s="23">
         <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="15">
+      <c r="A148" s="23">
         <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="15">
+      <c r="A149" s="23">
         <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="15">
+      <c r="A150" s="23">
         <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="15">
+      <c r="A151" s="23">
         <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="15">
+      <c r="A152" s="23">
         <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="15">
+      <c r="A153" s="23">
         <v>256</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="15">
+      <c r="A154" s="23">
         <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="15">
+      <c r="A155" s="23">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="15">
+      <c r="A156" s="23">
         <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="15">
+      <c r="A157" s="23">
         <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="15">
+      <c r="A158" s="23">
         <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="15">
+      <c r="A159" s="23">
         <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="15">
+      <c r="A160" s="23">
         <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="15">
+      <c r="A161" s="23">
         <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="15">
+      <c r="A162" s="23">
         <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="15">
+      <c r="A163" s="23">
         <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="15">
+      <c r="A164" s="23">
         <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="15">
+      <c r="A165" s="23">
         <v>268</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="15">
+      <c r="A166" s="23">
         <v>269</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="15">
+      <c r="A167" s="23">
         <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="15">
+      <c r="A168" s="23">
         <v>271</v>
       </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="15">
+      <c r="A169" s="23">
         <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="15">
+      <c r="A170" s="23">
         <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="15">
+      <c r="A171" s="23">
         <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="15">
+      <c r="A172" s="23">
         <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="15">
+      <c r="A173" s="23">
         <v>276</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="15">
+      <c r="A174" s="23">
         <v>277</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="15">
+      <c r="A175" s="23">
         <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="15">
+      <c r="A176" s="23">
         <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="15">
+      <c r="A177" s="23">
         <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="15">
+      <c r="A178" s="23">
         <v>281</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="15">
+      <c r="A179" s="23">
         <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="15">
+      <c r="A180" s="23">
         <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="15">
+      <c r="A181" s="23">
         <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="15">
+      <c r="A182" s="23">
         <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="15">
+      <c r="A183" s="23">
         <v>286</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="15">
+      <c r="A184" s="23">
         <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="15">
+      <c r="A185" s="23">
         <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="15">
+      <c r="A186" s="23">
         <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="15">
+      <c r="A187" s="23">
         <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="15">
+      <c r="A188" s="23">
         <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="15">
+      <c r="A189" s="23">
         <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="15">
+      <c r="A190" s="23">
         <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="15">
+      <c r="A191" s="23">
         <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="15">
+      <c r="A192" s="23">
         <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="15">
+      <c r="A193" s="23">
         <v>296</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="15">
+      <c r="A194" s="23">
         <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="15">
+      <c r="A195" s="23">
         <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="15">
+      <c r="A196" s="23">
         <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="15">
+      <c r="A197" s="23">
         <v>300</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="15">
+      <c r="A198" s="23">
         <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="15">
+      <c r="A199" s="23">
         <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="15">
+      <c r="A200" s="23">
         <v>303</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="15">
+      <c r="A201" s="23">
         <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="15">
+      <c r="A202" s="23">
         <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="15">
+      <c r="A203" s="23">
         <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="15">
+      <c r="A204" s="23">
         <v>307</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="15">
+      <c r="A205" s="23">
         <v>308</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="15">
+      <c r="A206" s="23">
         <v>309</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="15">
+      <c r="A207" s="23">
         <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="15">
+      <c r="A208" s="23">
         <v>311</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="15">
+      <c r="A209" s="23">
         <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="15">
+      <c r="A210" s="23">
         <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="15">
+      <c r="A211" s="23">
         <v>314</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="15">
+      <c r="A212" s="23">
         <v>315</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="15">
+      <c r="A213" s="23">
         <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="15">
+      <c r="A214" s="23">
         <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="15">
+      <c r="A215" s="23">
         <v>318</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="15">
+      <c r="A216" s="23">
         <v>319</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="15">
+      <c r="A217" s="23">
         <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="15">
+      <c r="A218" s="23">
         <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" s="15">
+      <c r="A219" s="23">
         <v>322</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="15">
+      <c r="A220" s="23">
         <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" s="15">
+      <c r="A221" s="23">
         <v>324</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="15">
+      <c r="A222" s="23">
         <v>325</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" s="15">
+      <c r="A223" s="23">
         <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="15">
+      <c r="A224" s="23">
         <v>327</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="15">
+      <c r="A225" s="23">
         <v>328</v>
       </c>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="15">
+      <c r="A226" s="23">
         <v>329</v>
       </c>
     </row>
     <row r="227" spans="1:1">
-      <c r="A227" s="15">
+      <c r="A227" s="23">
         <v>330</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="15">
+      <c r="A228" s="23">
         <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="15">
+      <c r="A229" s="23">
         <v>332</v>
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="15">
+      <c r="A230" s="23">
         <v>333</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="15">
+      <c r="A231" s="23">
         <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="15">
+      <c r="A232" s="23">
         <v>335</v>
       </c>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="15">
+      <c r="A233" s="23">
         <v>336</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="15">
+      <c r="A234" s="23">
         <v>337</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="15">
+      <c r="A235" s="23">
         <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="15">
+      <c r="A236" s="23">
         <v>339</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237" s="15">
+      <c r="A237" s="23">
         <v>340</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="15">
+      <c r="A238" s="23">
         <v>341</v>
       </c>
     </row>
     <row r="239" spans="1:1">
-      <c r="A239" s="15">
+      <c r="A239" s="23">
         <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="15">
+      <c r="A240" s="23">
         <v>343</v>
       </c>
     </row>
     <row r="241" spans="1:1">
-      <c r="A241" s="15">
+      <c r="A241" s="23">
         <v>344</v>
       </c>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="15">
+      <c r="A242" s="23">
         <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:1">
-      <c r="A243" s="15">
+      <c r="A243" s="23">
         <v>346</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="15">
+      <c r="A244" s="23">
         <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245" s="15">
+      <c r="A245" s="23">
         <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="15">
+      <c r="A246" s="23">
         <v>349</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" s="15">
+      <c r="A247" s="23">
         <v>350</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="15">
+      <c r="A248" s="23">
         <v>351</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" s="15">
+      <c r="A249" s="23">
         <v>352</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="15">
+      <c r="A250" s="23">
         <v>353</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" s="15">
+      <c r="A251" s="23">
         <v>354</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="15">
+      <c r="A252" s="23">
         <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:1">
-      <c r="A253" s="15">
+      <c r="A253" s="23">
         <v>356</v>
       </c>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="15">
+      <c r="A254" s="23">
         <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:1">
-      <c r="A255" s="15">
+      <c r="A255" s="23">
         <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="15">
+      <c r="A256" s="23">
         <v>359</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" s="15">
+      <c r="A257" s="23">
         <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="15">
+      <c r="A258" s="23">
         <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:1">
-      <c r="A259" s="15">
+      <c r="A259" s="23">
         <v>362</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="15">
+      <c r="A260" s="23">
         <v>363</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261" s="15">
+      <c r="A261" s="23">
         <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="15">
+      <c r="A262" s="23">
         <v>365</v>
       </c>
     </row>
@@ -2887,505 +3312,505 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="7.24271844660194" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.24271844660194" style="14" customWidth="1"/>
     <col min="2" max="2" width="20.9708737864078" customWidth="1"/>
     <col min="3" max="3" width="101.106796116505" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" spans="1:3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>19</v>
+    <row r="1" s="10" customFormat="1" spans="1:3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
-      <c r="A2" s="2">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
-      <c r="A4" s="2">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:2">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:3">
+      <c r="A6" s="14"/>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" s="10" customFormat="1" spans="1:3">
+      <c r="A7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:2">
-      <c r="A5" s="2">
+    <row r="8" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A8" s="19">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A9" s="19">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" s="18" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A10" s="19">
+        <v>3</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" s="18" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A11" s="19">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="C6" t="s">
+      <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A12" s="19">
+        <v>5</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" s="18" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A13" s="19">
+        <v>6</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A14" s="19">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A15" s="19">
+        <v>8</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" s="18" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A16" s="19">
+        <v>9</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" s="18" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A17" s="19">
+        <v>10</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" s="10" customFormat="1" spans="1:3">
+      <c r="A19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" s="7" customFormat="1" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A8" s="10">
+      <c r="C19" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="14">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="14">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="14">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="14">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="14">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="14">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" s="10" customFormat="1" spans="1:3">
+      <c r="A27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A9" s="10">
+      <c r="C27" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="14">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="14">
         <v>2</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" s="8" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A10" s="10">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="14">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="14">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="14">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="14">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="14">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="14">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="14">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="14">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" s="10" customFormat="1" spans="1:3">
+      <c r="A39" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" s="8" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A11" s="10">
+      <c r="C39" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="14">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="14">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="14">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="14">
         <v>4</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A12" s="10">
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="14">
         <v>5</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" s="8" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A13" s="10">
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="14">
         <v>6</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A14" s="10">
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="14">
         <v>7</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A15" s="10">
-        <v>8</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" s="8" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A16" s="10">
-        <v>9</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" s="8" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A17" s="10">
-        <v>10</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" s="7" customFormat="1" spans="1:3">
-      <c r="A19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" s="7" customFormat="1" spans="1:3">
-      <c r="A27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="2">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="2">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="2">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="2">
-        <v>10</v>
-      </c>
-      <c r="B37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" s="7" customFormat="1" spans="1:3">
-      <c r="A39" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="2">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="2">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="2">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="2">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="2">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="2">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="2">
-        <v>7</v>
-      </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3412,10 +3837,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3436,157 +3861,762 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.66019417475728" style="2"/>
-    <col min="2" max="2" width="33.2912621359223" style="3" customWidth="1"/>
-    <col min="3" max="3" width="78.1359223300971" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.66019417475728" style="2"/>
+    <col min="1" max="1" width="8.66019417475728" style="14"/>
+    <col min="2" max="2" width="33.2912621359223" style="15" customWidth="1"/>
+    <col min="3" max="3" width="78.1359223300971" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.66019417475728" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>19</v>
+    <row r="1" s="13" customFormat="1" spans="1:3">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>109</v>
+      <c r="B2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>111</v>
+      <c r="B3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" s="13" customFormat="1" spans="1:3">
+      <c r="A6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="15" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="15" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>116</v>
+      <c r="C8" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
+      <c r="C9" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" s="13" customFormat="1" spans="1:3">
+      <c r="A11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>119</v>
+      <c r="B12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>120</v>
+      <c r="B13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:3">
-      <c r="A16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
+      <c r="B14" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" s="13" customFormat="1" spans="1:3">
+      <c r="A16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="3" t="s">
-        <v>122</v>
+      <c r="B17" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" ht="77.15" spans="2:3">
-      <c r="B20" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>127</v>
+      <c r="B20" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" ht="46.3" spans="2:3">
-      <c r="B21" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>129</v>
+      <c r="B21" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="52.0485436893204" customWidth="1"/>
+    <col min="2" max="2" width="80.631067961165" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="9" customFormat="1" spans="1:1">
+      <c r="A1" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="1" spans="1:1">
+      <c r="A2" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" s="9" customFormat="1" spans="1:1">
+      <c r="A9" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" s="9" customFormat="1" spans="1:1">
+      <c r="A10" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" s="9" customFormat="1" spans="1:1">
+      <c r="A16" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:1">
+      <c r="A17" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" s="9" customFormat="1" spans="1:1">
+      <c r="A22" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" s="9" customFormat="1" spans="1:1">
+      <c r="A23" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" s="9" customFormat="1" spans="1:1">
+      <c r="A30" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" ht="15.45" spans="1:2">
+      <c r="A32" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4"/>
+  <cols>
+    <col min="1" max="1" width="51.252427184466" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:1">
+      <c r="A6" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:1">
+      <c r="A15" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="1" spans="1:1">
+      <c r="A16" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" s="4" customFormat="1" spans="1:1">
+      <c r="A20" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" s="4" customFormat="1" spans="1:1">
+      <c r="A24" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" s="4" customFormat="1" spans="1:1">
+      <c r="A28" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" customFormat="1" spans="1:1">
+      <c r="A29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" spans="1:1">
+      <c r="A30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" customFormat="1" spans="1:1">
+      <c r="A31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" s="4" customFormat="1" spans="1:1">
+      <c r="A36" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" customFormat="1" spans="1:1">
+      <c r="A37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" ht="14" customHeight="1"/>
+    <row r="41" s="3" customFormat="1" spans="1:1">
+      <c r="A41" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" s="4" customFormat="1" spans="1:1">
+      <c r="A42" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" customFormat="1" spans="1:1">
+      <c r="A43" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" customFormat="1" spans="1:1">
+      <c r="A44" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" customFormat="1" spans="1:1">
+      <c r="A45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" s="4" customFormat="1" spans="1:1">
+      <c r="A46" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" customFormat="1" spans="1:1">
+      <c r="A47" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" s="4" customFormat="1" spans="1:1">
+      <c r="A48" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" customFormat="1" spans="1:1">
+      <c r="A49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" s="4" customFormat="1" spans="1:1">
+      <c r="A50" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" ht="14" customHeight="1"/>
+    <row r="53" s="3" customFormat="1" spans="1:1">
+      <c r="A53" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" s="4" customFormat="1" spans="1:1">
+      <c r="A54" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" s="4" customFormat="1" spans="1:1">
+      <c r="A58" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" s="4" customFormat="1" spans="1:1">
+      <c r="A60" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" s="4" customFormat="1" spans="1:1">
+      <c r="A62" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" s="4" customFormat="1" spans="1:1">
+      <c r="A64" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:1">
+      <c r="A67" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" s="4" customFormat="1" spans="1:1">
+      <c r="A68" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" s="4" customFormat="1" spans="1:1">
+      <c r="A70" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" s="4" customFormat="1" spans="1:1">
+      <c r="A73" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="75" s="4" customFormat="1" spans="1:1">
+      <c r="A75" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="77" s="4" customFormat="1" spans="1:1">
+      <c r="A77" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" s="3" customFormat="1" spans="1:1">
+      <c r="A80" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" s="4" customFormat="1" spans="1:1">
+      <c r="A81" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" s="4" customFormat="1" spans="1:1">
+      <c r="A83" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" s="4" customFormat="1" spans="1:1">
+      <c r="A85" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" s="4" customFormat="1" spans="1:1">
+      <c r="A87" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
更新 main 專案 - 2025-12-29 00:03:15
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28740" windowHeight="13542"/>
+    <workbookView windowWidth="21882" windowHeight="11057"/>
   </bookViews>
   <sheets>
     <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250">
   <si>
     <t>Devlog</t>
   </si>
@@ -71,9 +71,6 @@
 樹精技能實現</t>
   </si>
   <si>
-    <t>小灰鳥技能位移</t>
-  </si>
-  <si>
     <t>開始按鈕太早按失效修復
 生成半徑太大偵測圓卡噸修復
 小灰鳥技能碰撞體實現</t>
@@ -82,16 +79,29 @@
     <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現</t>
   </si>
   <si>
+    <t>加入技能發動移動行為(1段-&gt;2段)
+史萊姆位移攻擊實現</t>
+  </si>
+  <si>
     <t>關卡通關、關卡失敗條件設定</t>
   </si>
   <si>
+    <t>SkillObject屬性移到SkillTemplate
+高度位移(重力)實作
+小灰鳥技能前後、高度位移
+小灰鳥持續攻擊動畫設置</t>
+  </si>
+  <si>
     <t>腳色死亡動畫重製</t>
   </si>
   <si>
     <t>腳色受傷動畫繪製</t>
   </si>
   <si>
-    <t>實際釋放技能後行為SkillDashType、SkillRecoveryType、DashSpeed、DashDuration、技能動畫分三段(中段持續循環)</t>
+    <t>史萊姆技能預置體設定</t>
+  </si>
+  <si>
+    <t>小灰鳥攻擊前預備動作位移</t>
   </si>
   <si>
     <t>攻擊要素</t>
@@ -518,6 +528,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <charset val="134"/>
+      </rPr>
       <t>收集、提煉參考參考</t>
     </r>
     <r>
@@ -525,6 +541,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FF1D41D5"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>(概念設計的真正內功)</t>
@@ -791,13 +808,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,6 +867,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -866,16 +898,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="新細明體"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -886,6 +918,20 @@
       <color theme="3"/>
       <name val="新細明體"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -905,7 +951,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
@@ -929,14 +989,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -951,7 +1004,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -965,40 +1018,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color rgb="FF1D41D5"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1022,31 +1046,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,37 +1082,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,7 +1112,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,7 +1130,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,79 +1220,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,6 +1237,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1240,15 +1279,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1266,11 +1296,29 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1289,181 +1337,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1477,23 +1501,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1508,9 +1520,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1899,1398 +1908,1405 @@
   <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.9805825242718" style="23" customWidth="1"/>
-    <col min="2" max="2" width="72.2330097087379" style="23" customWidth="1"/>
-    <col min="3" max="3" width="105.766990291262" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="23"/>
+    <col min="1" max="1" width="12.9805825242718" style="18" customWidth="1"/>
+    <col min="2" max="2" width="72.2330097087379" style="18" customWidth="1"/>
+    <col min="3" max="3" width="105.766990291262" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" s="22" customFormat="1" ht="18.45" spans="1:3">
-      <c r="A1" s="22" t="s">
+    <row r="1" s="17" customFormat="1" ht="18.45" spans="1:3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="36.85" spans="1:3">
-      <c r="A2" s="23">
+      <c r="A2" s="18">
         <v>105</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="18.45" spans="1:3">
-      <c r="A3" s="23">
+      <c r="A3" s="18">
         <v>106</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="36.85" spans="1:3">
-      <c r="A4" s="23">
+      <c r="A4" s="18">
         <v>107</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="18.45" spans="1:3">
-      <c r="A5" s="23">
+      <c r="A5" s="18">
         <v>108</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="18.45" spans="1:3">
-      <c r="A6" s="23">
+      <c r="A6" s="18">
         <v>109</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" ht="36.85" spans="1:3">
-      <c r="A7" s="23">
+      <c r="A7" s="18">
         <v>110</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" ht="18.45" spans="1:2">
-      <c r="A8" s="23">
+      <c r="A8" s="18">
         <v>111</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="55.3" spans="1:3">
-      <c r="A9" s="23">
+      <c r="A9" s="18">
         <v>112</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" ht="55.3" spans="1:3">
+      <c r="A10" s="18">
+        <v>113</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" ht="55.3" spans="1:3">
-      <c r="A10" s="23">
-        <v>113</v>
-      </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="26" t="s">
+    </row>
+    <row r="11" ht="36.85" spans="1:3">
+      <c r="A11" s="18">
+        <v>114</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" ht="18.45" spans="1:3">
-      <c r="A11" s="23">
-        <v>114</v>
-      </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" ht="18.45" spans="1:3">
-      <c r="A12" s="23">
+    <row r="12" ht="73.7" spans="1:3">
+      <c r="A12" s="18">
         <v>115</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="22" t="s">
         <v>20</v>
       </c>
+      <c r="C12" s="22" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" ht="18.45" spans="1:3">
-      <c r="A13" s="23">
+      <c r="A13" s="18">
         <v>116</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" ht="36.85" spans="1:3">
-      <c r="A14" s="23">
+      <c r="B13" s="18"/>
+      <c r="C13" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" ht="18.45" spans="1:3">
+      <c r="A14" s="18">
         <v>117</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23">
+      <c r="C14" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" ht="18.45" spans="1:3">
+      <c r="A15" s="18">
         <v>118</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="22" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="23">
+      <c r="A16" s="18">
         <v>119</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="22"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="23">
+      <c r="A17" s="18">
         <v>120</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="22"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="23">
+      <c r="A18" s="18">
         <v>121</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="22"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="23">
+      <c r="A19" s="18">
         <v>122</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="22"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="23">
+      <c r="A20" s="18">
         <v>123</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="22"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="23">
+      <c r="A21" s="18">
         <v>124</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="22"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="23">
+      <c r="A22" s="18">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="23">
+      <c r="A23" s="18">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="23">
+      <c r="A24" s="18">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="23">
+      <c r="A25" s="18">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="23">
+      <c r="A26" s="18">
         <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="23">
+      <c r="A27" s="18">
         <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="23">
+      <c r="A28" s="18">
         <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="23">
+      <c r="A29" s="18">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="23">
+      <c r="A30" s="18">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="23">
+      <c r="A31" s="18">
         <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="23">
+      <c r="A32" s="18">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="23">
+      <c r="A33" s="18">
         <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="23">
+      <c r="A34" s="18">
         <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="23">
+      <c r="A35" s="18">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="23">
+      <c r="A36" s="18">
         <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="23">
+      <c r="A37" s="18">
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="23">
+      <c r="A38" s="18">
         <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="23">
+      <c r="A39" s="18">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="23">
+      <c r="A40" s="18">
         <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="23">
+      <c r="A41" s="18">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="23">
+      <c r="A42" s="18">
         <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="23">
+      <c r="A43" s="18">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="23">
+      <c r="A44" s="18">
         <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="23">
+      <c r="A45" s="18">
         <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="23">
+      <c r="A46" s="18">
         <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="23">
+      <c r="A47" s="18">
         <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="23">
+      <c r="A48" s="18">
         <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="23">
+      <c r="A49" s="18">
         <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="23">
+      <c r="A50" s="18">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="23">
+      <c r="A51" s="18">
         <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="23">
+      <c r="A52" s="18">
         <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="23">
+      <c r="A53" s="18">
         <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="23">
+      <c r="A54" s="18">
         <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="23">
+      <c r="A55" s="18">
         <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="23">
+      <c r="A56" s="18">
         <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="23">
+      <c r="A57" s="18">
         <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="23">
+      <c r="A58" s="18">
         <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="23">
+      <c r="A59" s="18">
         <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="23">
+      <c r="A60" s="18">
         <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="23">
+      <c r="A61" s="18">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="23">
+      <c r="A62" s="18">
         <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="23">
+      <c r="A63" s="18">
         <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="23">
+      <c r="A64" s="18">
         <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="23">
+      <c r="A65" s="18">
         <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="23">
+      <c r="A66" s="18">
         <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="23">
+      <c r="A67" s="18">
         <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="23">
+      <c r="A68" s="18">
         <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="23">
+      <c r="A69" s="18">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="23">
+      <c r="A70" s="18">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="23">
+      <c r="A71" s="18">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="23">
+      <c r="A72" s="18">
         <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="23">
+      <c r="A73" s="18">
         <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="23">
+      <c r="A74" s="18">
         <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="23">
+      <c r="A75" s="18">
         <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="23">
+      <c r="A76" s="18">
         <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="23">
+      <c r="A77" s="18">
         <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="23">
+      <c r="A78" s="18">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="23">
+      <c r="A79" s="18">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="23">
+      <c r="A80" s="18">
         <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="23">
+      <c r="A81" s="18">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="23">
+      <c r="A82" s="18">
         <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="23">
+      <c r="A83" s="18">
         <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="23">
+      <c r="A84" s="18">
         <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="23">
+      <c r="A85" s="18">
         <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="23">
+      <c r="A86" s="18">
         <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="23">
+      <c r="A87" s="18">
         <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="23">
+      <c r="A88" s="18">
         <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="23">
+      <c r="A89" s="18">
         <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="23">
+      <c r="A90" s="18">
         <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="23">
+      <c r="A91" s="18">
         <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="23">
+      <c r="A92" s="18">
         <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="23">
+      <c r="A93" s="18">
         <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="23">
+      <c r="A94" s="18">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="23">
+      <c r="A95" s="18">
         <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="23">
+      <c r="A96" s="18">
         <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="23">
+      <c r="A97" s="18">
         <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="23">
+      <c r="A98" s="18">
         <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="23">
+      <c r="A99" s="18">
         <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="23">
+      <c r="A100" s="18">
         <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="23">
+      <c r="A101" s="18">
         <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="23">
+      <c r="A102" s="18">
         <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="23">
+      <c r="A103" s="18">
         <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="23">
+      <c r="A104" s="18">
         <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="23">
+      <c r="A105" s="18">
         <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="23">
+      <c r="A106" s="18">
         <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="23">
+      <c r="A107" s="18">
         <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="23">
+      <c r="A108" s="18">
         <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="23">
+      <c r="A109" s="18">
         <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="23">
+      <c r="A110" s="18">
         <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="23">
+      <c r="A111" s="18">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="23">
+      <c r="A112" s="18">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="23">
+      <c r="A113" s="18">
         <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="23">
+      <c r="A114" s="18">
         <v>217</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="23">
+      <c r="A115" s="18">
         <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="23">
+      <c r="A116" s="18">
         <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="23">
+      <c r="A117" s="18">
         <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="23">
+      <c r="A118" s="18">
         <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="23">
+      <c r="A119" s="18">
         <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="23">
+      <c r="A120" s="18">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="23">
+      <c r="A121" s="18">
         <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="23">
+      <c r="A122" s="18">
         <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="23">
+      <c r="A123" s="18">
         <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="23">
+      <c r="A124" s="18">
         <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="23">
+      <c r="A125" s="18">
         <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="23">
+      <c r="A126" s="18">
         <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="23">
+      <c r="A127" s="18">
         <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="23">
+      <c r="A128" s="18">
         <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="23">
+      <c r="A129" s="18">
         <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="23">
+      <c r="A130" s="18">
         <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="23">
+      <c r="A131" s="18">
         <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="23">
+      <c r="A132" s="18">
         <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="23">
+      <c r="A133" s="18">
         <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="23">
+      <c r="A134" s="18">
         <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="23">
+      <c r="A135" s="18">
         <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="23">
+      <c r="A136" s="18">
         <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="23">
+      <c r="A137" s="18">
         <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="23">
+      <c r="A138" s="18">
         <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="23">
+      <c r="A139" s="18">
         <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="23">
+      <c r="A140" s="18">
         <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="23">
+      <c r="A141" s="18">
         <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="23">
+      <c r="A142" s="18">
         <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="23">
+      <c r="A143" s="18">
         <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="23">
+      <c r="A144" s="18">
         <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="23">
+      <c r="A145" s="18">
         <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="23">
+      <c r="A146" s="18">
         <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="23">
+      <c r="A147" s="18">
         <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="23">
+      <c r="A148" s="18">
         <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="23">
+      <c r="A149" s="18">
         <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="23">
+      <c r="A150" s="18">
         <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="23">
+      <c r="A151" s="18">
         <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="23">
+      <c r="A152" s="18">
         <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="23">
+      <c r="A153" s="18">
         <v>256</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="23">
+      <c r="A154" s="18">
         <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="23">
+      <c r="A155" s="18">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="23">
+      <c r="A156" s="18">
         <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="23">
+      <c r="A157" s="18">
         <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="23">
+      <c r="A158" s="18">
         <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="23">
+      <c r="A159" s="18">
         <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="23">
+      <c r="A160" s="18">
         <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="23">
+      <c r="A161" s="18">
         <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="23">
+      <c r="A162" s="18">
         <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="23">
+      <c r="A163" s="18">
         <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="23">
+      <c r="A164" s="18">
         <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="23">
+      <c r="A165" s="18">
         <v>268</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="23">
+      <c r="A166" s="18">
         <v>269</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="23">
+      <c r="A167" s="18">
         <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="23">
+      <c r="A168" s="18">
         <v>271</v>
       </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="23">
+      <c r="A169" s="18">
         <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="23">
+      <c r="A170" s="18">
         <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="23">
+      <c r="A171" s="18">
         <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="23">
+      <c r="A172" s="18">
         <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="23">
+      <c r="A173" s="18">
         <v>276</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="23">
+      <c r="A174" s="18">
         <v>277</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="23">
+      <c r="A175" s="18">
         <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="23">
+      <c r="A176" s="18">
         <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="23">
+      <c r="A177" s="18">
         <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="23">
+      <c r="A178" s="18">
         <v>281</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="23">
+      <c r="A179" s="18">
         <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="23">
+      <c r="A180" s="18">
         <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="23">
+      <c r="A181" s="18">
         <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="23">
+      <c r="A182" s="18">
         <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="23">
+      <c r="A183" s="18">
         <v>286</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="23">
+      <c r="A184" s="18">
         <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="23">
+      <c r="A185" s="18">
         <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="23">
+      <c r="A186" s="18">
         <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="23">
+      <c r="A187" s="18">
         <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="23">
+      <c r="A188" s="18">
         <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="23">
+      <c r="A189" s="18">
         <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="23">
+      <c r="A190" s="18">
         <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="23">
+      <c r="A191" s="18">
         <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="23">
+      <c r="A192" s="18">
         <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="23">
+      <c r="A193" s="18">
         <v>296</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="23">
+      <c r="A194" s="18">
         <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="23">
+      <c r="A195" s="18">
         <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="23">
+      <c r="A196" s="18">
         <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="23">
+      <c r="A197" s="18">
         <v>300</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="23">
+      <c r="A198" s="18">
         <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="23">
+      <c r="A199" s="18">
         <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="23">
+      <c r="A200" s="18">
         <v>303</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="23">
+      <c r="A201" s="18">
         <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="23">
+      <c r="A202" s="18">
         <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="23">
+      <c r="A203" s="18">
         <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="23">
+      <c r="A204" s="18">
         <v>307</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="23">
+      <c r="A205" s="18">
         <v>308</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="23">
+      <c r="A206" s="18">
         <v>309</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="23">
+      <c r="A207" s="18">
         <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="23">
+      <c r="A208" s="18">
         <v>311</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="23">
+      <c r="A209" s="18">
         <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="23">
+      <c r="A210" s="18">
         <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="23">
+      <c r="A211" s="18">
         <v>314</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="23">
+      <c r="A212" s="18">
         <v>315</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="23">
+      <c r="A213" s="18">
         <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="23">
+      <c r="A214" s="18">
         <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="23">
+      <c r="A215" s="18">
         <v>318</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="23">
+      <c r="A216" s="18">
         <v>319</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="23">
+      <c r="A217" s="18">
         <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="23">
+      <c r="A218" s="18">
         <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" s="23">
+      <c r="A219" s="18">
         <v>322</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="23">
+      <c r="A220" s="18">
         <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" s="23">
+      <c r="A221" s="18">
         <v>324</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="23">
+      <c r="A222" s="18">
         <v>325</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" s="23">
+      <c r="A223" s="18">
         <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="23">
+      <c r="A224" s="18">
         <v>327</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="23">
+      <c r="A225" s="18">
         <v>328</v>
       </c>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="23">
+      <c r="A226" s="18">
         <v>329</v>
       </c>
     </row>
     <row r="227" spans="1:1">
-      <c r="A227" s="23">
+      <c r="A227" s="18">
         <v>330</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="23">
+      <c r="A228" s="18">
         <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="23">
+      <c r="A229" s="18">
         <v>332</v>
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="23">
+      <c r="A230" s="18">
         <v>333</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="23">
+      <c r="A231" s="18">
         <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="23">
+      <c r="A232" s="18">
         <v>335</v>
       </c>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="23">
+      <c r="A233" s="18">
         <v>336</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="23">
+      <c r="A234" s="18">
         <v>337</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="23">
+      <c r="A235" s="18">
         <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="23">
+      <c r="A236" s="18">
         <v>339</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237" s="23">
+      <c r="A237" s="18">
         <v>340</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="23">
+      <c r="A238" s="18">
         <v>341</v>
       </c>
     </row>
     <row r="239" spans="1:1">
-      <c r="A239" s="23">
+      <c r="A239" s="18">
         <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="23">
+      <c r="A240" s="18">
         <v>343</v>
       </c>
     </row>
     <row r="241" spans="1:1">
-      <c r="A241" s="23">
+      <c r="A241" s="18">
         <v>344</v>
       </c>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="23">
+      <c r="A242" s="18">
         <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:1">
-      <c r="A243" s="23">
+      <c r="A243" s="18">
         <v>346</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="23">
+      <c r="A244" s="18">
         <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245" s="23">
+      <c r="A245" s="18">
         <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="23">
+      <c r="A246" s="18">
         <v>349</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" s="23">
+      <c r="A247" s="18">
         <v>350</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="23">
+      <c r="A248" s="18">
         <v>351</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" s="23">
+      <c r="A249" s="18">
         <v>352</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="23">
+      <c r="A250" s="18">
         <v>353</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" s="23">
+      <c r="A251" s="18">
         <v>354</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="23">
+      <c r="A252" s="18">
         <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:1">
-      <c r="A253" s="23">
+      <c r="A253" s="18">
         <v>356</v>
       </c>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="23">
+      <c r="A254" s="18">
         <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:1">
-      <c r="A255" s="23">
+      <c r="A255" s="18">
         <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="23">
+      <c r="A256" s="18">
         <v>359</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" s="23">
+      <c r="A257" s="18">
         <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="23">
+      <c r="A258" s="18">
         <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:1">
-      <c r="A259" s="23">
+      <c r="A259" s="18">
         <v>362</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="23">
+      <c r="A260" s="18">
         <v>363</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261" s="23">
+      <c r="A261" s="18">
         <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="23">
+      <c r="A262" s="18">
         <v>365</v>
       </c>
     </row>
@@ -3312,505 +3328,505 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="7.24271844660194" style="14" customWidth="1"/>
+    <col min="1" max="1" width="7.24271844660194" style="10" customWidth="1"/>
     <col min="2" max="2" width="20.9708737864078" customWidth="1"/>
     <col min="3" max="3" width="101.106796116505" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" spans="1:3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>24</v>
+    <row r="1" s="6" customFormat="1" spans="1:3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:2">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:3">
+      <c r="A6" s="10"/>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" s="6" customFormat="1" spans="1:3">
+      <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:3">
-      <c r="A4" s="14">
+    </row>
+    <row r="8" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A10" s="14">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" s="13" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A11" s="14">
+        <v>4</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A12" s="14">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" s="13" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A13" s="14">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A14" s="14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A15" s="14">
+        <v>8</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" s="13" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A16" s="14">
+        <v>9</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" s="13" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A17" s="14">
+        <v>10</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" s="6" customFormat="1" spans="1:3">
+      <c r="A19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:2">
-      <c r="A5" s="14">
+      <c r="C19" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="10">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="10">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="10">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" s="6" customFormat="1" spans="1:3">
+      <c r="A27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:3">
-      <c r="A6" s="14"/>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" s="10" customFormat="1" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="C27" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="10">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="10">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="10">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="10">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="10">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="10">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="10">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="10">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" s="6" customFormat="1" spans="1:3">
+      <c r="A39" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A8" s="19">
+      <c r="C39" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="10">
         <v>1</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A9" s="19">
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="10">
         <v>2</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" s="18" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A10" s="19">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" s="18" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A11" s="19">
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="10">
         <v>4</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A12" s="19">
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" s="18" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A13" s="19">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A14" s="19">
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="10">
         <v>7</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A15" s="19">
-        <v>8</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" s="18" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A16" s="19">
-        <v>9</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" s="18" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A17" s="19">
-        <v>10</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" s="10" customFormat="1" spans="1:3">
-      <c r="A19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="14">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="14">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="14">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="14">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="14">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="14">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" s="10" customFormat="1" spans="1:3">
-      <c r="A27" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="14">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="14">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="14">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="14">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="14">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="14">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="14">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="14">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="14">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="14">
-        <v>10</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" s="10" customFormat="1" spans="1:3">
-      <c r="A39" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="14">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="14">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="14">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="14">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="14">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="14">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="14">
-        <v>7</v>
-      </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3837,10 +3853,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3861,157 +3877,157 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.66019417475728" style="14"/>
-    <col min="2" max="2" width="33.2912621359223" style="15" customWidth="1"/>
-    <col min="3" max="3" width="78.1359223300971" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.66019417475728" style="14"/>
+    <col min="1" max="1" width="8.66019417475728" style="10"/>
+    <col min="2" max="2" width="33.2912621359223" style="7" customWidth="1"/>
+    <col min="3" max="3" width="78.1359223300971" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="8.66019417475728" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" spans="1:3">
-      <c r="A1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>24</v>
+    <row r="1" s="9" customFormat="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>114</v>
+      <c r="B2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="1" spans="1:3">
+      <c r="A6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="15" t="s">
+      <c r="C7" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" s="13" customFormat="1" spans="1:3">
-      <c r="A6" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="C8" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="15" t="s">
+      <c r="C9" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" s="9" customFormat="1" spans="1:3">
+      <c r="A11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="15" t="s">
+      <c r="C12" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" s="13" customFormat="1" spans="1:3">
-      <c r="A11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>125</v>
+      <c r="C13" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" s="13" customFormat="1" spans="1:3">
-      <c r="A16" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>24</v>
+      <c r="B14" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" s="9" customFormat="1" spans="1:3">
+      <c r="A16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="15" t="s">
-        <v>127</v>
+      <c r="B17" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" ht="77.15" spans="2:3">
-      <c r="B20" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>132</v>
+      <c r="B20" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="21" ht="46.3" spans="2:3">
-      <c r="B21" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>134</v>
+      <c r="B21" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4035,161 +4051,161 @@
     <col min="2" max="2" width="80.631067961165" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" spans="1:1">
-      <c r="A1" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" s="9" customFormat="1" spans="1:1">
-      <c r="A2" s="10" t="s">
-        <v>136</v>
+    <row r="1" s="6" customFormat="1" spans="1:1">
+      <c r="A1" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" s="6" customFormat="1" spans="1:1">
+      <c r="A2" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" s="9" customFormat="1" spans="1:1">
-      <c r="A9" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" s="9" customFormat="1" spans="1:1">
-      <c r="A10" s="10" t="s">
         <v>143</v>
       </c>
     </row>
+    <row r="9" s="6" customFormat="1" spans="1:1">
+      <c r="A9" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" s="6" customFormat="1" spans="1:1">
+      <c r="A10" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="6" t="s">
-        <v>144</v>
+      <c r="A11" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="6" t="s">
-        <v>145</v>
+      <c r="A12" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="6" t="s">
-        <v>146</v>
+      <c r="A13" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" s="9" customFormat="1" spans="1:1">
-      <c r="A16" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="1" spans="1:1">
+      <c r="A16" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:1">
-      <c r="A17" s="6" t="s">
-        <v>149</v>
+      <c r="A17" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="6" t="s">
-        <v>150</v>
+      <c r="A18" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="6" t="s">
-        <v>151</v>
+      <c r="A19" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" s="9" customFormat="1" spans="1:1">
-      <c r="A22" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" s="9" customFormat="1" spans="1:1">
-      <c r="A23" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="22" s="6" customFormat="1" spans="1:1">
+      <c r="A22" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" s="6" customFormat="1" spans="1:1">
+      <c r="A23" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="6" t="s">
-        <v>155</v>
+      <c r="A24" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="6" t="s">
-        <v>156</v>
+      <c r="A25" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="6" t="s">
-        <v>157</v>
+      <c r="A26" s="5" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" s="9" customFormat="1" spans="1:1">
-      <c r="A30" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" s="6" customFormat="1" spans="1:1">
+      <c r="A30" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" ht="15.45" spans="1:2">
-      <c r="A32" s="12" t="s">
-        <v>162</v>
+      <c r="A32" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="12" t="s">
-        <v>164</v>
+      <c r="A33" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4213,410 +4229,410 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
-      <c r="A1" s="5" t="s">
-        <v>168</v>
+      <c r="A1" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
-        <v>170</v>
+      <c r="A4" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="6" t="s">
-        <v>171</v>
+      <c r="A5" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:1">
-      <c r="A6" s="6" t="s">
-        <v>172</v>
+      <c r="A6" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="6" t="s">
-        <v>174</v>
+      <c r="A8" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="6" t="s">
-        <v>175</v>
+      <c r="A9" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="6" t="s">
-        <v>177</v>
+      <c r="A11" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="6" t="s">
-        <v>178</v>
+      <c r="A12" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="6" t="s">
-        <v>179</v>
+      <c r="A13" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:1">
-      <c r="A15" s="7" t="s">
-        <v>180</v>
+      <c r="A15" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:1">
-      <c r="A16" s="8" t="s">
-        <v>181</v>
+      <c r="A16" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:1">
-      <c r="A20" s="8" t="s">
-        <v>185</v>
+      <c r="A20" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="1" spans="1:1">
-      <c r="A24" s="8" t="s">
-        <v>185</v>
+      <c r="A24" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" s="4" customFormat="1" spans="1:1">
-      <c r="A28" s="8" t="s">
-        <v>192</v>
+      <c r="A28" s="4" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:1">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:1">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:1">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" s="4" customFormat="1" spans="1:1">
-      <c r="A36" s="8" t="s">
-        <v>200</v>
+      <c r="A36" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:1">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" ht="14" customHeight="1"/>
     <row r="41" s="3" customFormat="1" spans="1:1">
-      <c r="A41" s="7" t="s">
-        <v>204</v>
+      <c r="A41" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="42" s="4" customFormat="1" spans="1:1">
       <c r="A42" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:1">
       <c r="A43" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:1">
       <c r="A44" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:1">
       <c r="A45" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" s="4" customFormat="1" spans="1:1">
       <c r="A46" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:1">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" s="4" customFormat="1" spans="1:1">
       <c r="A48" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:1">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" s="4" customFormat="1" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1"/>
     <row r="53" s="3" customFormat="1" spans="1:1">
-      <c r="A53" s="7" t="s">
-        <v>215</v>
+      <c r="A53" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="54" s="4" customFormat="1" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" s="4" customFormat="1" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" s="4" customFormat="1" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" s="4" customFormat="1" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" s="4" customFormat="1" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="67" s="3" customFormat="1" spans="1:1">
-      <c r="A67" s="7" t="s">
-        <v>227</v>
+      <c r="A67" s="3" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="68" s="4" customFormat="1" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" s="4" customFormat="1" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" s="4" customFormat="1" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="75" s="4" customFormat="1" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77" s="4" customFormat="1" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="1" spans="1:1">
-      <c r="A80" s="7" t="s">
-        <v>239</v>
+      <c r="A80" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="81" s="4" customFormat="1" spans="1:1">
       <c r="A81" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" s="4" customFormat="1" spans="1:1">
       <c r="A83" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" s="4" customFormat="1" spans="1:1">
       <c r="A85" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" s="4" customFormat="1" spans="1:1">
       <c r="A87" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Devlog116 - 2025-12-30 00:15:07
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246">
   <si>
     <t>Devlog</t>
   </si>
@@ -76,14 +76,8 @@
 小灰鳥技能碰撞體實現</t>
   </si>
   <si>
-    <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現</t>
-  </si>
-  <si>
     <t>加入技能發動移動行為(1段-&gt;2段)
 史萊姆位移攻擊實現</t>
-  </si>
-  <si>
-    <t>關卡通關、關卡失敗條件設定</t>
   </si>
   <si>
     <t>SkillObject屬性移到SkillTemplate
@@ -92,16 +86,17 @@
 小灰鳥持續攻擊動畫設置</t>
   </si>
   <si>
-    <t>腳色死亡動畫重製</t>
-  </si>
-  <si>
-    <t>腳色受傷動畫繪製</t>
-  </si>
-  <si>
-    <t>史萊姆技能預置體設定</t>
-  </si>
-  <si>
-    <t>小灰鳥攻擊前預備動作位移</t>
+    <t>史萊姆技能預置體設定完成
+準備攻擊動畫事件入口完成
+小灰鳥準備動作位移-&gt;衝刺攻擊(Skill01-&gt;Skill01-1)
+水平衝刺位移問題修正(SkillDashing順序問題，被StopCoroutine關掉了)</t>
+  </si>
+  <si>
+    <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現
+腳色受傷動畫繪製
+腳色死亡動畫重製
+關卡通關、關卡失敗條件設定
+評估近戰攻擊不使用生成物，直接在腳色身上啟用，需要解決高度問題判定問題，應該跟主物件同步Todo</t>
   </si>
   <si>
     <t>攻擊要素</t>
@@ -808,13 +803,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,16 +862,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="新細明體"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,6 +892,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -907,7 +908,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,14 +923,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -951,6 +952,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -960,14 +962,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,15 +983,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1010,12 +999,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1046,7 +1047,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,7 +1197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,79 +1209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1154,79 +1221,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,17 +1241,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1279,17 +1280,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1314,15 +1309,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1337,75 +1323,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1414,76 +1415,76 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1907,8 +1908,8 @@
   <sheetPr/>
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
@@ -2018,56 +2019,48 @@
       <c r="B10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" ht="36.85" spans="1:3">
       <c r="A11" s="18">
         <v>114</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C11" s="22"/>
     </row>
     <row r="12" ht="73.7" spans="1:3">
       <c r="A12" s="18">
         <v>115</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" ht="18.45" spans="1:3">
+      <c r="B12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" ht="110.55" spans="1:3">
       <c r="A13" s="18">
         <v>116</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="22" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" ht="18.45" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="18">
         <v>117</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" ht="18.45" spans="1:3">
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="18">
         <v>118</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="C15" s="22"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="18">
@@ -3336,10 +3329,10 @@
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="9"/>
       <c r="B1" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
@@ -3347,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
@@ -3355,10 +3348,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -3366,10 +3359,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:2">
@@ -3377,24 +3370,24 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
       <c r="A6" s="10"/>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:3">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3402,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3410,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" s="13" customFormat="1" ht="15.45" spans="1:3">
@@ -3418,10 +3411,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" s="13" customFormat="1" ht="15.45" spans="1:3">
@@ -3429,10 +3422,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3440,7 +3433,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" s="13" customFormat="1" ht="15.45" spans="1:3">
@@ -3448,10 +3441,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3459,7 +3452,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3467,7 +3460,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" s="13" customFormat="1" ht="15.45" spans="1:3">
@@ -3475,10 +3468,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" s="13" customFormat="1" ht="15.45" spans="1:2">
@@ -3486,18 +3479,18 @@
         <v>10</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" s="6" customFormat="1" spans="1:3">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3505,10 +3498,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3516,10 +3509,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3527,10 +3520,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3538,10 +3531,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3549,10 +3542,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3560,18 +3553,18 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" s="6" customFormat="1" spans="1:3">
       <c r="A27" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3579,10 +3572,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3590,7 +3583,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -3598,10 +3591,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3609,10 +3602,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3620,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3628,10 +3621,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3639,10 +3632,10 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3650,10 +3643,10 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3661,10 +3654,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3672,21 +3665,21 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" s="6" customFormat="1" spans="1:3">
       <c r="A39" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3694,10 +3687,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -3705,10 +3698,10 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3716,10 +3709,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -3727,10 +3720,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3738,73 +3731,73 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -3812,10 +3805,10 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -3823,10 +3816,10 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3853,10 +3846,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3885,149 +3878,149 @@
   <sheetData>
     <row r="1" s="9" customFormat="1" spans="1:3">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="1" spans="1:3">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" s="9" customFormat="1" spans="1:3">
       <c r="A16" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" ht="77.15" spans="2:3">
       <c r="B20" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" ht="46.3" spans="2:3">
       <c r="B21" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4053,159 +4046,159 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" s="6" customFormat="1" spans="1:1">
       <c r="A9" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="1" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" s="6" customFormat="1" spans="1:1">
       <c r="A16" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="1" spans="1:1">
       <c r="A22" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" s="6" customFormat="1" spans="1:1">
       <c r="A23" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" s="6" customFormat="1" spans="1:1">
       <c r="A30" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" ht="15.45" spans="1:2">
       <c r="A32" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4230,409 +4223,409 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:1">
       <c r="A6" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:1">
       <c r="A15" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:1">
       <c r="A16" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:1">
       <c r="A20" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="1" spans="1:1">
       <c r="A24" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" s="4" customFormat="1" spans="1:1">
       <c r="A28" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:1">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:1">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:1">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" s="4" customFormat="1" spans="1:1">
       <c r="A36" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:1">
       <c r="A37" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" ht="14" customHeight="1"/>
     <row r="41" s="3" customFormat="1" spans="1:1">
       <c r="A41" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" s="4" customFormat="1" spans="1:1">
       <c r="A42" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:1">
       <c r="A43" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:1">
       <c r="A44" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:1">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" s="4" customFormat="1" spans="1:1">
       <c r="A46" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:1">
       <c r="A47" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" s="4" customFormat="1" spans="1:1">
       <c r="A48" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:1">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" s="4" customFormat="1" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1"/>
     <row r="53" s="3" customFormat="1" spans="1:1">
       <c r="A53" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" s="4" customFormat="1" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" s="4" customFormat="1" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" s="4" customFormat="1" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" s="4" customFormat="1" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" s="4" customFormat="1" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" s="3" customFormat="1" spans="1:1">
       <c r="A67" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" s="4" customFormat="1" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" s="4" customFormat="1" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" s="4" customFormat="1" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" s="4" customFormat="1" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" s="4" customFormat="1" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="1" spans="1:1">
       <c r="A80" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" s="4" customFormat="1" spans="1:1">
       <c r="A81" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" s="4" customFormat="1" spans="1:1">
       <c r="A83" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" s="4" customFormat="1" spans="1:1">
       <c r="A85" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" s="4" customFormat="1" spans="1:1">
       <c r="A87" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day118 - 2026-01-01 00:06:24
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21882" windowHeight="11057"/>
+    <workbookView windowWidth="21882" windowHeight="10800" tabRatio="621"/>
   </bookViews>
   <sheets>
     <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
-    <sheet name="攻擊" sheetId="2" r:id="rId2"/>
-    <sheet name="動畫設計" sheetId="3" r:id="rId3"/>
-    <sheet name="場景規劃" sheetId="4" r:id="rId4"/>
-    <sheet name="概念設計" sheetId="5" r:id="rId5"/>
+    <sheet name="概念設計" sheetId="2" r:id="rId2"/>
+    <sheet name="場景規劃" sheetId="3" r:id="rId3"/>
+    <sheet name="尺寸、Layer參數設定" sheetId="4" r:id="rId4"/>
+    <sheet name="動畫設計" sheetId="5" r:id="rId5"/>
     <sheet name="設計關鍵字" sheetId="6" r:id="rId6"/>
+    <sheet name="攻擊" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262">
   <si>
     <t>Devlog</t>
   </si>
@@ -86,359 +87,49 @@
 小灰鳥持續攻擊動畫設置</t>
   </si>
   <si>
+    <t>概念：
+城牆用核心設計，累積受損值會提高城鎮的成本，通過新關卡後會解除，這可以用來作為遊戲難度的平衡使用</t>
+  </si>
+  <si>
     <t>史萊姆技能預置體設定完成
 準備攻擊動畫事件入口完成
 小灰鳥準備動作位移-&gt;衝刺攻擊(Skill01-&gt;Skill01-1)
 水平衝刺位移問題修正(SkillDashing順序問題，被StopCoroutine關掉了)</t>
   </si>
   <si>
-    <t>空中敵人的碰撞體調整，底部碰撞體可被穿越。or 小鳥技能的實現
+    <t>程式：
+通關後等待一下才允許點擊返回
+通關後結算畫面
+掉落物系統
+背包系統
 腳色受傷動畫繪製
 腳色死亡動畫重製
-關卡通關、關卡失敗條件設定
-評估近戰攻擊不使用生成物，直接在腳色身上啟用，需要解決高度問題判定問題，應該跟主物件同步Todo</t>
-  </si>
-  <si>
-    <t>攻擊要素</t>
-  </si>
-  <si>
-    <t>備註</t>
-  </si>
-  <si>
-    <t>時機</t>
-  </si>
-  <si>
-    <t>接近性</t>
-  </si>
-  <si>
-    <t>距離</t>
-  </si>
-  <si>
-    <t>併發性</t>
-  </si>
-  <si>
-    <t>最複雜多樣化的部分、大幅的影響遊戲體驗及遊戲平衡性，限制、控制敵方每秒傷害的總和</t>
-  </si>
-  <si>
-    <t>方向(攻擊、攝像機)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>一</t>
-  </si>
-  <si>
-    <t>對目標感知</t>
-  </si>
-  <si>
-    <t>攻擊方向</t>
-  </si>
-  <si>
-    <t>攻擊者分配</t>
-  </si>
-  <si>
-    <t>管理系統</t>
-  </si>
-  <si>
-    <t>選擇行動</t>
-  </si>
-  <si>
-    <t>根據狀態、規則、其他要素或隨機。</t>
-  </si>
-  <si>
-    <t>行動準備</t>
-  </si>
-  <si>
-    <t>預期框架</t>
-  </si>
-  <si>
-    <t>可識別行動</t>
-  </si>
-  <si>
-    <t>命中幀</t>
-  </si>
-  <si>
-    <t>攻擊間格幀</t>
-  </si>
-  <si>
-    <t>解析度幀</t>
-  </si>
-  <si>
-    <t>恢復平衡</t>
-  </si>
-  <si>
-    <t>恢復到待機</t>
-  </si>
-  <si>
-    <t>二</t>
-  </si>
-  <si>
-    <t>近戰攻擊</t>
-  </si>
-  <si>
-    <t>攻擊位移</t>
-  </si>
-  <si>
-    <t>遠距攻擊</t>
-  </si>
-  <si>
-    <t>範圍顯示、特效顯示</t>
-  </si>
-  <si>
-    <t>空間大小</t>
-  </si>
-  <si>
-    <t>小:距離近，大:距離遠</t>
-  </si>
-  <si>
-    <t>障礙物</t>
-  </si>
-  <si>
-    <t>掩體、窄道、大型障礙物</t>
-  </si>
-  <si>
-    <t>移動限制</t>
-  </si>
-  <si>
-    <t>地塊破壞、速度影響</t>
-  </si>
-  <si>
-    <t>陷阱物件</t>
-  </si>
-  <si>
-    <t>三</t>
-  </si>
-  <si>
-    <t>1V1決鬥V2甚至V3</t>
-  </si>
-  <si>
-    <t>Boss戰，截然不同的遊戲體驗，與普通敵人強大的對比</t>
-  </si>
-  <si>
-    <t>1V多</t>
-  </si>
-  <si>
-    <t>免費攻擊者遊戲</t>
-  </si>
-  <si>
-    <t>無高階系統控制、限制多敵人時的攻擊頻率</t>
-  </si>
-  <si>
-    <t>攻擊票</t>
-  </si>
-  <si>
-    <t>玩家戰鬥體驗變得可控、避免玩家不知所措。難度提高可提高敵人攻擊頻率</t>
-  </si>
-  <si>
-    <t>敵人來襲數量票</t>
-  </si>
-  <si>
-    <t>敵人種類區分</t>
-  </si>
-  <si>
-    <t>普通敵人(可預測)、高階敵人(複雜、挑戰性)有特別標示比如紅框、金框、籃框、綠框)</t>
-  </si>
-  <si>
-    <t>生存類</t>
-  </si>
-  <si>
-    <t>被敵人淹沒、不使用攻擊票、使用控制敵人生成數量</t>
-  </si>
-  <si>
-    <t>合作類</t>
-  </si>
-  <si>
-    <t>分散攻擊目標</t>
-  </si>
-  <si>
-    <t>混亂程度</t>
-  </si>
-  <si>
-    <t>小:更容易被解析</t>
-  </si>
-  <si>
-    <t>可控性</t>
-  </si>
-  <si>
-    <t>控制得越少，就越有即時感</t>
-  </si>
-  <si>
-    <t>四</t>
-  </si>
-  <si>
-    <t>視角</t>
-  </si>
-  <si>
-    <t>第一人稱、第三人稱、側視、俯視</t>
-  </si>
-  <si>
-    <t>俯視、側視</t>
-  </si>
-  <si>
-    <t>考慮同時顯示所有具威脅性敵人</t>
-  </si>
-  <si>
-    <t>螢幕外攻擊</t>
-  </si>
-  <si>
-    <t>預警提示(重要性有待評估)</t>
-  </si>
-  <si>
-    <t>攝影機風格</t>
-  </si>
-  <si>
-    <t>影響場景設計</t>
-  </si>
-  <si>
-    <t>受擊狀態</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>畏縮flinch</t>
-  </si>
-  <si>
-    <t>被打瞬間的小退縮、抖一下、不位移</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>踉蹌stumble</t>
-  </si>
-  <si>
-    <t>身體失衡、後退一步</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>硬直hitstun</t>
-  </si>
-  <si>
-    <t>不能動、不能出招</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>擊退knockback</t>
-  </si>
-  <si>
-    <t>被推飛一段距離</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>擊倒knockdown</t>
-  </si>
-  <si>
-    <t>倒地(較長時間)</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>浮空airborne</t>
-  </si>
-  <si>
-    <t>被打飛到空中</t>
-  </si>
-  <si>
-    <t>安排敵人位置</t>
-  </si>
-  <si>
-    <t>有利於訓練玩家控制能力</t>
-  </si>
-  <si>
-    <t>螢幕外的攻擊</t>
-  </si>
-  <si>
-    <t>讓玩家感覺並非無敵、降低掌控感</t>
-  </si>
-  <si>
-    <t>戰士大招</t>
-  </si>
-  <si>
-    <t>連續劈斬*5，大橫斬*1</t>
-  </si>
-  <si>
-    <t>遠景</t>
-  </si>
-  <si>
-    <t>顏色</t>
-  </si>
-  <si>
-    <t>飽和低、對比低</t>
-  </si>
-  <si>
-    <t>細節</t>
-  </si>
-  <si>
-    <t>幾乎沒線條感</t>
-  </si>
-  <si>
-    <t>大小</t>
-  </si>
-  <si>
-    <t>物件比中景大且模糊</t>
-  </si>
-  <si>
-    <t>中景</t>
-  </si>
-  <si>
-    <t>飽和中、別太亮、地面比角色暗一點</t>
-  </si>
-  <si>
-    <t>輪廓清楚</t>
-  </si>
-  <si>
-    <t>物件符合角色比例</t>
-  </si>
-  <si>
-    <t>前景</t>
-  </si>
-  <si>
-    <t>比中景更暗、偏同色系、透明度50-80</t>
-  </si>
-  <si>
-    <t>邊角、偶爾、別出現在腳色臉上</t>
-  </si>
-  <si>
-    <t>調色</t>
-  </si>
-  <si>
-    <t>主色系(80%物件同色系)</t>
-  </si>
-  <si>
-    <t>黃綠（溫暖、安全）</t>
-  </si>
-  <si>
-    <t>藍綠（神秘、深林）</t>
-  </si>
-  <si>
-    <t>冷灰綠（危險、敵多）</t>
-  </si>
-  <si>
-    <t>飽和度</t>
-  </si>
-  <si>
-    <t>玩家最高
-敵人高
-中景中
-前景中偏低
-遠景低</t>
-  </si>
-  <si>
-    <t>物件數量</t>
-  </si>
-  <si>
-    <t>大物件(樹木、瀑布1-2)
-中物件(橋、遺跡2-3)
-小物件(草、蘑菇)自由</t>
+關卡失敗條件設定</t>
+  </si>
+  <si>
+    <t>繪製草坪、草群
+場景結構前、中、後景分配
+風格確認
+樹木試繪
+SkillObject實作SkillHeightComponent(重力效果待實測)
+近戰附著攻擊類型已實作高度跟隨腳色
+底部Move Collider已可不互相碰撞</t>
+  </si>
+  <si>
+    <t>美術：
+城防結界核心
+前景灌木叢、中景土地、灌木叢中景樹木、遠景樹林、山脈繪製
+先看概念設計、場景規劃</t>
+  </si>
+  <si>
+    <t>草地雜訊、泥土雜訊、邊界密度、行動空間留白、邊界草20-30%布置完成
+腳色被擊非、擊退異常修復
+玩家攻擊面向修復
+技能方向修復
+重力修復
+弓箭手技能修復
+衝刺中被攻擊會無法行動修復
+通關條件新增：關卡敵人總數殲滅</t>
   </si>
   <si>
     <t>訓練法一：世界拆解練習（每天 15–30 分）</t>
@@ -558,6 +249,141 @@
     <t>大量專業的知識儲備</t>
   </si>
   <si>
+    <t>一</t>
+  </si>
+  <si>
+    <t>遠景</t>
+  </si>
+  <si>
+    <t>備註</t>
+  </si>
+  <si>
+    <t>顏色</t>
+  </si>
+  <si>
+    <t>飽和低、對比低</t>
+  </si>
+  <si>
+    <t>細節</t>
+  </si>
+  <si>
+    <t>幾乎沒線條感</t>
+  </si>
+  <si>
+    <t>大小</t>
+  </si>
+  <si>
+    <t>物件比中景大且模糊</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>中景</t>
+  </si>
+  <si>
+    <t>飽和中、別太亮、地面比角色暗一點</t>
+  </si>
+  <si>
+    <t>輪廓清楚</t>
+  </si>
+  <si>
+    <t>物件符合角色比例</t>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>前景</t>
+  </si>
+  <si>
+    <t>比中景更暗、偏同色系、透明度50-80</t>
+  </si>
+  <si>
+    <t>邊角、偶爾、別出現在腳色臉上</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>調色</t>
+  </si>
+  <si>
+    <t>主色系(80%物件同色系)</t>
+  </si>
+  <si>
+    <t>黃綠（溫暖、安全）</t>
+  </si>
+  <si>
+    <t>藍綠（神秘、深林）</t>
+  </si>
+  <si>
+    <t>冷灰綠（危險、敵多）</t>
+  </si>
+  <si>
+    <t>飽和度</t>
+  </si>
+  <si>
+    <t>玩家最高
+敵人高
+中景中
+前景中偏低
+遠景低</t>
+  </si>
+  <si>
+    <t>物件數量</t>
+  </si>
+  <si>
+    <t>大物件(樹木、瀑布1-2)
+中物件(橋、遺跡2-3)
+小物件(草、蘑菇)自由</t>
+  </si>
+  <si>
+    <t>高</t>
+  </si>
+  <si>
+    <t>寬</t>
+  </si>
+  <si>
+    <t>PPU</t>
+  </si>
+  <si>
+    <t>Sorting Layer</t>
+  </si>
+  <si>
+    <t>主角</t>
+  </si>
+  <si>
+    <t>場景</t>
+  </si>
+  <si>
+    <t>遠景前可互動物件</t>
+  </si>
+  <si>
+    <t>DetectorSpriteSpawner</t>
+  </si>
+  <si>
+    <t>腳色BackSprite</t>
+  </si>
+  <si>
+    <t>陰影</t>
+  </si>
+  <si>
+    <t>中景中可互動物件</t>
+  </si>
+  <si>
+    <t>玩家、敵人、樹木、建築、物件</t>
+  </si>
+  <si>
+    <t>邊界框</t>
+  </si>
+  <si>
+    <t>戰士大招</t>
+  </si>
+  <si>
+    <t>連續劈斬*5，大橫斬*1</t>
+  </si>
+  <si>
     <t>分類不適想更多，而是「敢刪除」，選3-5個分類點，明確「不選什麼」</t>
   </si>
   <si>
@@ -771,9 +597,6 @@
     <t>一看就懂/需要解讀/誤導性外觀</t>
   </si>
   <si>
-    <t>場景</t>
-  </si>
-  <si>
     <t>空間層級</t>
   </si>
   <si>
@@ -796,6 +619,252 @@
   </si>
   <si>
     <t>安全區/壓迫區/神秘區/過度區</t>
+  </si>
+  <si>
+    <t>攻擊要素</t>
+  </si>
+  <si>
+    <t>時機</t>
+  </si>
+  <si>
+    <t>接近性</t>
+  </si>
+  <si>
+    <t>距離</t>
+  </si>
+  <si>
+    <t>併發性</t>
+  </si>
+  <si>
+    <t>最複雜多樣化的部分、大幅的影響遊戲體驗及遊戲平衡性，限制、控制敵方每秒傷害的總和</t>
+  </si>
+  <si>
+    <t>方向(攻擊、攝像機)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>對目標感知</t>
+  </si>
+  <si>
+    <t>攻擊方向</t>
+  </si>
+  <si>
+    <t>攻擊者分配</t>
+  </si>
+  <si>
+    <t>管理系統</t>
+  </si>
+  <si>
+    <t>選擇行動</t>
+  </si>
+  <si>
+    <t>根據狀態、規則、其他要素或隨機。</t>
+  </si>
+  <si>
+    <t>行動準備</t>
+  </si>
+  <si>
+    <t>預期框架</t>
+  </si>
+  <si>
+    <t>可識別行動</t>
+  </si>
+  <si>
+    <t>命中幀</t>
+  </si>
+  <si>
+    <t>攻擊間格幀</t>
+  </si>
+  <si>
+    <t>解析度幀</t>
+  </si>
+  <si>
+    <t>恢復平衡</t>
+  </si>
+  <si>
+    <t>恢復到待機</t>
+  </si>
+  <si>
+    <t>近戰攻擊</t>
+  </si>
+  <si>
+    <t>攻擊位移</t>
+  </si>
+  <si>
+    <t>遠距攻擊</t>
+  </si>
+  <si>
+    <t>範圍顯示、特效顯示</t>
+  </si>
+  <si>
+    <t>空間大小</t>
+  </si>
+  <si>
+    <t>小:距離近，大:距離遠</t>
+  </si>
+  <si>
+    <t>障礙物</t>
+  </si>
+  <si>
+    <t>掩體、窄道、大型障礙物</t>
+  </si>
+  <si>
+    <t>移動限制</t>
+  </si>
+  <si>
+    <t>地塊破壞、速度影響</t>
+  </si>
+  <si>
+    <t>陷阱物件</t>
+  </si>
+  <si>
+    <t>1V1決鬥V2甚至V3</t>
+  </si>
+  <si>
+    <t>Boss戰，截然不同的遊戲體驗，與普通敵人強大的對比</t>
+  </si>
+  <si>
+    <t>1V多</t>
+  </si>
+  <si>
+    <t>免費攻擊者遊戲</t>
+  </si>
+  <si>
+    <t>無高階系統控制、限制多敵人時的攻擊頻率</t>
+  </si>
+  <si>
+    <t>攻擊票</t>
+  </si>
+  <si>
+    <t>玩家戰鬥體驗變得可控、避免玩家不知所措。難度提高可提高敵人攻擊頻率</t>
+  </si>
+  <si>
+    <t>敵人來襲數量票</t>
+  </si>
+  <si>
+    <t>敵人種類區分</t>
+  </si>
+  <si>
+    <t>普通敵人(可預測)、高階敵人(複雜、挑戰性)有特別標示比如紅框、金框、籃框、綠框)</t>
+  </si>
+  <si>
+    <t>生存類</t>
+  </si>
+  <si>
+    <t>被敵人淹沒、不使用攻擊票、使用控制敵人生成數量</t>
+  </si>
+  <si>
+    <t>合作類</t>
+  </si>
+  <si>
+    <t>分散攻擊目標</t>
+  </si>
+  <si>
+    <t>混亂程度</t>
+  </si>
+  <si>
+    <t>小:更容易被解析</t>
+  </si>
+  <si>
+    <t>可控性</t>
+  </si>
+  <si>
+    <t>控制得越少，就越有即時感</t>
+  </si>
+  <si>
+    <t>視角</t>
+  </si>
+  <si>
+    <t>第一人稱、第三人稱、側視、俯視</t>
+  </si>
+  <si>
+    <t>俯視、側視</t>
+  </si>
+  <si>
+    <t>考慮同時顯示所有具威脅性敵人</t>
+  </si>
+  <si>
+    <t>螢幕外攻擊</t>
+  </si>
+  <si>
+    <t>預警提示(重要性有待評估)</t>
+  </si>
+  <si>
+    <t>攝影機風格</t>
+  </si>
+  <si>
+    <t>影響場景設計</t>
+  </si>
+  <si>
+    <t>受擊狀態</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>畏縮flinch</t>
+  </si>
+  <si>
+    <t>被打瞬間的小退縮、抖一下、不位移</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>踉蹌stumble</t>
+  </si>
+  <si>
+    <t>身體失衡、後退一步</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>硬直hitstun</t>
+  </si>
+  <si>
+    <t>不能動、不能出招</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>擊退knockback</t>
+  </si>
+  <si>
+    <t>被推飛一段距離</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>擊倒knockdown</t>
+  </si>
+  <si>
+    <t>倒地(較長時間)</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>浮空airborne</t>
+  </si>
+  <si>
+    <t>被打飛到空中</t>
+  </si>
+  <si>
+    <t>安排敵人位置</t>
+  </si>
+  <si>
+    <t>有利於訓練玩家控制能力</t>
+  </si>
+  <si>
+    <t>螢幕外的攻擊</t>
+  </si>
+  <si>
+    <t>讓玩家感覺並非無敵、降低掌控感</t>
   </si>
 </sst>
 </file>
@@ -803,14 +872,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="29">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -829,14 +906,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -870,7 +939,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -907,8 +983,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,15 +999,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -954,15 +1025,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -985,14 +1055,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
@@ -1000,7 +1062,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1008,6 +1070,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1047,13 +1116,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,43 +1200,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,31 +1218,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1155,55 +1284,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1215,19 +1296,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,16 +1311,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1282,9 +1351,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1294,32 +1365,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1338,6 +1383,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1346,145 +1415,145 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1492,53 +1561,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1908,8 +1977,8 @@
   <sheetPr/>
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
@@ -2037,28 +2106,38 @@
       <c r="B12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" ht="110.55" spans="1:3">
+      <c r="C12" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" ht="147.45" spans="1:3">
       <c r="A13" s="18">
         <v>116</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" ht="129" spans="1:3">
       <c r="A14" s="18">
         <v>117</v>
       </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" ht="165.85" spans="1:3">
       <c r="A15" s="18">
         <v>118</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -3313,523 +3392,488 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="7.24271844660194" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.9708737864078" customWidth="1"/>
-    <col min="3" max="3" width="101.106796116505" customWidth="1"/>
+    <col min="1" max="1" width="52.0485436893204" customWidth="1"/>
+    <col min="2" max="2" width="80.631067961165" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="1" spans="1:2">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="1" spans="1:3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:3">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="2" s="1" customFormat="1" spans="1:1">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:2">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" customFormat="1" spans="1:3">
-      <c r="A6" s="10"/>
-      <c r="C6" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="1" spans="1:3">
-      <c r="A7" s="9" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A8" s="14">
-        <v>1</v>
-      </c>
-      <c r="B8" s="13" t="s">
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A9" s="14">
-        <v>2</v>
-      </c>
-      <c r="B9" s="13" t="s">
+    <row r="9" s="1" customFormat="1" spans="1:1">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" s="13" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A10" s="14">
-        <v>3</v>
-      </c>
-      <c r="B10" s="13" t="s">
+    <row r="10" s="1" customFormat="1" spans="1:1">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="13" t="s">
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" s="13" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A11" s="14">
-        <v>4</v>
-      </c>
-      <c r="B11" s="13" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="13" t="s">
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A12" s="14">
-        <v>5</v>
-      </c>
-      <c r="B12" s="13" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" s="13" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A13" s="14">
-        <v>6</v>
-      </c>
-      <c r="B13" s="13" t="s">
+    <row r="16" s="1" customFormat="1" spans="1:1">
+      <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="13" t="s">
+    </row>
+    <row r="17" customFormat="1" spans="1:1">
+      <c r="A17" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A14" s="14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="13" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A15" s="14">
-        <v>8</v>
-      </c>
-      <c r="B15" s="13" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="1" ht="15.45" spans="1:3">
-      <c r="A16" s="14">
-        <v>9</v>
-      </c>
-      <c r="B16" s="13" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="13" t="s">
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:1">
+      <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" s="13" customFormat="1" ht="15.45" spans="1:2">
-      <c r="A17" s="14">
-        <v>10</v>
-      </c>
-      <c r="B17" s="13" t="s">
+    <row r="23" s="1" customFormat="1" spans="1:1">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" s="6" customFormat="1" spans="1:3">
-      <c r="A19" s="9" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="10">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="30" s="1" customFormat="1" spans="1:1">
+      <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="10">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="10">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="32" ht="15.45" spans="1:2">
+      <c r="A32" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="10">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" s="6" customFormat="1" spans="1:3">
-      <c r="A27" s="9" t="s">
+      <c r="B34" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="10">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="10">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="10">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="10">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="10">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="10">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="10">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="10">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="10">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="10">
-        <v>10</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" s="6" customFormat="1" spans="1:3">
-      <c r="A39" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="10">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="10">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="10">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="10">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="10">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="10">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="10">
-        <v>7</v>
-      </c>
-      <c r="B52" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" t="s">
-        <v>107</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="8.66019417475728" style="3"/>
+    <col min="2" max="2" width="33.2912621359223" style="13" customWidth="1"/>
+    <col min="3" max="3" width="78.1359223300971" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.66019417475728" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="1" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="1" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="1" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" ht="77.15" spans="2:3">
+      <c r="B20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" ht="46.3" spans="2:3">
+      <c r="B21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4"/>
+  <cols>
+    <col min="6" max="6" width="14.9708737864078" customWidth="1"/>
+    <col min="7" max="7" width="13.3300970873786" customWidth="1"/>
+    <col min="8" max="8" width="21.2912621359223" customWidth="1"/>
+    <col min="10" max="10" width="34.1165048543689" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10">
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <f>11.5*B2</f>
+        <v>322</v>
+      </c>
+      <c r="C3">
+        <f>13*C2</f>
+        <v>572</v>
+      </c>
+      <c r="D3">
+        <v>572</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="4" spans="8:9">
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="5" spans="8:9">
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="8:10">
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6">
+        <v>-10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" ht="14" customHeight="1" spans="8:10">
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="8:9">
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="8:9">
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A2:B2"/>
@@ -3846,363 +3890,15 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" width="8.66019417475728" style="10"/>
-    <col min="2" max="2" width="33.2912621359223" style="7" customWidth="1"/>
-    <col min="3" max="3" width="78.1359223300971" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="8.66019417475728" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="9" customFormat="1" spans="1:3">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="1" spans="1:3">
-      <c r="A6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" s="9" customFormat="1" spans="1:3">
-      <c r="A11" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" s="9" customFormat="1" spans="1:3">
-      <c r="A16" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" ht="77.15" spans="2:3">
-      <c r="B20" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" ht="46.3" spans="2:3">
-      <c r="B21" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:B34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="52.0485436893204" customWidth="1"/>
-    <col min="2" max="2" width="80.631067961165" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:1">
-      <c r="A1" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" s="6" customFormat="1" spans="1:1">
-      <c r="A2" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" s="6" customFormat="1" spans="1:1">
-      <c r="A9" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" s="6" customFormat="1" spans="1:1">
-      <c r="A10" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" s="6" customFormat="1" spans="1:1">
-      <c r="A16" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" customFormat="1" spans="1:1">
-      <c r="A17" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" s="6" customFormat="1" spans="1:1">
-      <c r="A22" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" s="6" customFormat="1" spans="1:1">
-      <c r="A23" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" s="6" customFormat="1" spans="1:1">
-      <c r="A30" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" ht="15.45" spans="1:2">
-      <c r="A32" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B32" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>164</v>
-      </c>
-      <c r="B34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -4213,7 +3909,7 @@
   <dimension ref="A1:A88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4"/>
@@ -4221,415 +3917,934 @@
     <col min="1" max="1" width="51.252427184466" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>167</v>
+    <row r="1" s="8" customFormat="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" spans="1:1">
+      <c r="A3" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
-        <v>168</v>
+      <c r="A4" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5" t="s">
-        <v>169</v>
+      <c r="A5" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:1">
-      <c r="A6" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" s="2" customFormat="1" spans="1:1">
-      <c r="A7" s="2" t="s">
-        <v>171</v>
+      <c r="A6" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="1" spans="1:1">
+      <c r="A7" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
-        <v>172</v>
+      <c r="A8" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>174</v>
+      <c r="A9" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" s="9" customFormat="1" spans="1:1">
+      <c r="A10" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="5" t="s">
-        <v>175</v>
+      <c r="A11" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="5" t="s">
-        <v>176</v>
+      <c r="A12" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:1">
-      <c r="A15" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" s="4" customFormat="1" spans="1:1">
-      <c r="A16" s="4" t="s">
-        <v>179</v>
+      <c r="A13" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" s="10" customFormat="1" spans="1:1">
+      <c r="A15" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" s="11" customFormat="1" spans="1:1">
+      <c r="A16" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" s="4" customFormat="1" spans="1:1">
-      <c r="A20" s="4" t="s">
-        <v>183</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" s="11" customFormat="1" spans="1:1">
+      <c r="A20" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" s="4" customFormat="1" spans="1:1">
-      <c r="A24" s="4" t="s">
-        <v>183</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" s="11" customFormat="1" spans="1:1">
+      <c r="A24" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" s="4" customFormat="1" spans="1:1">
-      <c r="A28" s="4" t="s">
-        <v>190</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" s="11" customFormat="1" spans="1:1">
+      <c r="A28" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:1">
       <c r="A29" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:1">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:1">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="36" s="4" customFormat="1" spans="1:1">
-      <c r="A36" s="4" t="s">
-        <v>198</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" s="11" customFormat="1" spans="1:1">
+      <c r="A36" s="11" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:1">
       <c r="A37" t="s">
-        <v>199</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" ht="14" customHeight="1"/>
-    <row r="41" s="3" customFormat="1" spans="1:1">
-      <c r="A41" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" s="4" customFormat="1" spans="1:1">
-      <c r="A42" s="4" t="s">
-        <v>203</v>
+    <row r="41" s="10" customFormat="1" spans="1:1">
+      <c r="A41" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" s="11" customFormat="1" spans="1:1">
+      <c r="A42" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:1">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:1">
       <c r="A44" t="s">
-        <v>205</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:1">
       <c r="A45" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" s="4" customFormat="1" spans="1:1">
-      <c r="A46" s="4" t="s">
-        <v>207</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" s="11" customFormat="1" spans="1:1">
+      <c r="A46" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:1">
       <c r="A47" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="48" s="4" customFormat="1" spans="1:1">
-      <c r="A48" s="4" t="s">
-        <v>209</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" s="11" customFormat="1" spans="1:1">
+      <c r="A48" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:1">
       <c r="A49" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="50" s="4" customFormat="1" spans="1:1">
-      <c r="A50" s="4" t="s">
-        <v>211</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" s="11" customFormat="1" spans="1:1">
+      <c r="A50" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1"/>
-    <row r="53" s="3" customFormat="1" spans="1:1">
-      <c r="A53" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54" s="4" customFormat="1" spans="1:1">
-      <c r="A54" s="4" t="s">
-        <v>214</v>
+    <row r="53" s="10" customFormat="1" spans="1:1">
+      <c r="A53" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" s="11" customFormat="1" spans="1:1">
+      <c r="A54" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="58" s="4" customFormat="1" spans="1:1">
-      <c r="A58" s="4" t="s">
-        <v>218</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" s="11" customFormat="1" spans="1:1">
+      <c r="A58" s="11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="60" s="4" customFormat="1" spans="1:1">
-      <c r="A60" s="4" t="s">
-        <v>220</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" s="11" customFormat="1" spans="1:1">
+      <c r="A60" s="11" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62" s="4" customFormat="1" spans="1:1">
-      <c r="A62" s="4" t="s">
-        <v>222</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" s="11" customFormat="1" spans="1:1">
+      <c r="A62" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="64" s="4" customFormat="1" spans="1:1">
-      <c r="A64" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:1">
-      <c r="A67" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="68" s="4" customFormat="1" spans="1:1">
-      <c r="A68" s="4" t="s">
-        <v>226</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" s="11" customFormat="1" spans="1:1">
+      <c r="A64" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" s="10" customFormat="1" spans="1:1">
+      <c r="A67" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" s="11" customFormat="1" spans="1:1">
+      <c r="A68" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="70" s="4" customFormat="1" spans="1:1">
-      <c r="A70" s="4" t="s">
-        <v>228</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" s="11" customFormat="1" spans="1:1">
+      <c r="A70" s="11" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>229</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" s="4" customFormat="1" spans="1:1">
-      <c r="A73" s="4" t="s">
-        <v>231</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" s="11" customFormat="1" spans="1:1">
+      <c r="A73" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="75" s="4" customFormat="1" spans="1:1">
-      <c r="A75" s="4" t="s">
-        <v>233</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" s="11" customFormat="1" spans="1:1">
+      <c r="A75" s="11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="77" s="4" customFormat="1" spans="1:1">
-      <c r="A77" s="4" t="s">
-        <v>235</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" s="11" customFormat="1" spans="1:1">
+      <c r="A77" s="11" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="80" s="3" customFormat="1" spans="1:1">
-      <c r="A80" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="81" s="4" customFormat="1" spans="1:1">
-      <c r="A81" s="4" t="s">
-        <v>238</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" s="10" customFormat="1" spans="1:1">
+      <c r="A80" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" s="11" customFormat="1" spans="1:1">
+      <c r="A81" s="11" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="83" s="4" customFormat="1" spans="1:1">
-      <c r="A83" s="4" t="s">
-        <v>240</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" s="11" customFormat="1" spans="1:1">
+      <c r="A83" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="85" s="4" customFormat="1" spans="1:1">
-      <c r="A85" s="4" t="s">
-        <v>242</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" s="11" customFormat="1" spans="1:1">
+      <c r="A85" s="11" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="87" s="4" customFormat="1" spans="1:1">
-      <c r="A87" s="4" t="s">
-        <v>244</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" s="11" customFormat="1" spans="1:1">
+      <c r="A87" s="11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="7.24271844660194" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.9708737864078" customWidth="1"/>
+    <col min="3" max="3" width="101.106796116505" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="15.45" spans="1:3">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="15.45" spans="1:2">
+      <c r="A17" s="5">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" s="1" customFormat="1" spans="1:3">
+      <c r="A39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="3">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" t="s">
+        <v>241</v>
+      </c>
+      <c r="C45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" t="s">
+        <v>244</v>
+      </c>
+      <c r="C46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B47" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B48" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B49" t="s">
+        <v>253</v>
+      </c>
+      <c r="C49" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B50" t="s">
+        <v>256</v>
+      </c>
+      <c r="C50" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="3">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>260</v>
+      </c>
+      <c r="C52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Day119 - 2026-01-04 11:46:10
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21882" windowHeight="10800" tabRatio="621"/>
+    <workbookView windowWidth="21882" windowHeight="11057" tabRatio="621" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282">
   <si>
     <t>Devlog</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>敵人血量HpSlider修正</t>
+  </si>
+  <si>
+    <t>輸入指定按鍵，啟用特殊模式、商店、強化、裝備等等</t>
   </si>
   <si>
     <t>玩家及敵人攻擊面向修正
@@ -72,13 +75,35 @@
 樹精技能實現</t>
   </si>
   <si>
+    <t>要的不是「刺激」，
+要的是：陪伴感、旅途感、正在前進的感覺。
+這種音樂只會在一種遊戲裡成立——
+👉 玩家知道自己在一段旅程裡</t>
+  </si>
+  <si>
     <t>開始按鈕太早按失效修復
 生成半徑太大偵測圓卡噸修復
 小灰鳥技能碰撞體實現</t>
   </si>
   <si>
+    <t>因為現在很多遊戲是在做：
+系統疊加 → 認知負擔
+選項變多 → 決策疲勞
+世界變大 → 情感變薄
+而你要做的是反過來：
+縮小選擇範圍，放大每一個選擇的重量</t>
+  </si>
+  <si>
     <t>加入技能發動移動行為(1段-&gt;2段)
 史萊姆位移攻擊實現</t>
+  </si>
+  <si>
+    <t>Fun:必然可達成
+Appeal:置重點於吸引，可降低效率問題
+Scope:完成作品效率
+Monetization:先不考慮
+找到自己的遊戲定位!
+ps.透過幻想，實作些有趣但容易的遊戲尋找靈感(「縮減」影響核心體驗的內容，避免奪走注意力)</t>
   </si>
   <si>
     <t>SkillObject屬性移到SkillTemplate
@@ -98,7 +123,6 @@
   </si>
   <si>
     <t>程式：
-通關後等待一下才允許點擊返回
 通關後結算畫面
 掉落物系統
 背包系統
@@ -130,6 +154,15 @@
 弓箭手技能修復
 衝刺中被攻擊會無法行動修復
 通關條件新增：關卡敵人總數殲滅</t>
+  </si>
+  <si>
+    <t>遊戲場景切換問題排除。
+通關後等待一下才允許點擊返回，完成</t>
+  </si>
+  <si>
+    <t xml:space="preserve">四個敵人依照32PPU，飽和度30上下，重繪
+Sprite pivot底部客製高度完成
+</t>
   </si>
   <si>
     <t>訓練法一：世界拆解練習（每天 15–30 分）</t>
@@ -339,6 +372,12 @@
 小物件(草、蘑菇)自由</t>
   </si>
   <si>
+    <t>尺寸</t>
+  </si>
+  <si>
+    <t>Sorting Layer</t>
+  </si>
+  <si>
     <t>高</t>
   </si>
   <si>
@@ -348,18 +387,15 @@
     <t>PPU</t>
   </si>
   <si>
-    <t>Sorting Layer</t>
-  </si>
-  <si>
     <t>主角</t>
   </si>
   <si>
+    <t>遠景前可互動物件</t>
+  </si>
+  <si>
     <t>場景</t>
   </si>
   <si>
-    <t>遠景前可互動物件</t>
-  </si>
-  <si>
     <t>DetectorSpriteSpawner</t>
   </si>
   <si>
@@ -375,9 +411,55 @@
     <t>玩家、敵人、樹木、建築、物件</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
     <t>邊界框</t>
   </si>
   <si>
+    <t>60-80(70)</t>
+  </si>
+  <si>
+    <t>臉、武器、裝備焦點局部</t>
+  </si>
+  <si>
+    <t>敵人</t>
+  </si>
+  <si>
+    <t>45-60(50)</t>
+  </si>
+  <si>
+    <t>色相有差異
+不要跟背景同色系</t>
+  </si>
+  <si>
+    <t>15-35(20)</t>
+  </si>
+  <si>
+    <t>35-55(40)</t>
+  </si>
+  <si>
+    <t>偏灰、偏霧、像舞台布幕</t>
+  </si>
+  <si>
+    <t>物品</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>陰影強度</t>
+  </si>
+  <si>
+    <t>透明度HSV</t>
+  </si>
+  <si>
+    <t>一般情況</t>
+  </si>
+  <si>
     <t>戰士大招</t>
   </si>
   <si>
@@ -492,9 +574,6 @@
     <t>神聖/世俗/異質</t>
   </si>
   <si>
-    <t>敵人</t>
-  </si>
-  <si>
     <t>起源</t>
   </si>
   <si>
@@ -559,9 +638,6 @@
   </si>
   <si>
     <t>象徵性</t>
-  </si>
-  <si>
-    <t>物品</t>
   </si>
   <si>
     <t>功能性</t>
@@ -872,11 +948,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -939,14 +1015,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -957,6 +1026,13 @@
       <color theme="3"/>
       <name val="新細明體"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -983,9 +1059,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1001,7 +1076,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,16 +1105,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1055,28 +1136,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1116,49 +1192,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1170,49 +1234,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,7 +1258,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,49 +1360,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1296,7 +1372,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1310,17 +1386,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1345,26 +1415,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1402,8 +1452,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1412,152 +1488,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1598,6 +1674,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1626,6 +1708,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1977,1408 +2065,1429 @@
   <sheetPr/>
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.9805825242718" style="18" customWidth="1"/>
-    <col min="2" max="2" width="72.2330097087379" style="18" customWidth="1"/>
-    <col min="3" max="3" width="105.766990291262" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="18"/>
+    <col min="1" max="1" width="12.9805825242718" style="20" customWidth="1"/>
+    <col min="2" max="2" width="72.2330097087379" style="20" customWidth="1"/>
+    <col min="3" max="3" width="105.766990291262" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="1" ht="18.45" spans="1:3">
-      <c r="A1" s="17" t="s">
+    <row r="1" s="19" customFormat="1" ht="18.45" spans="1:3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="36.85" spans="1:3">
-      <c r="A2" s="18">
+      <c r="A2" s="20">
         <v>105</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="18.45" spans="1:3">
-      <c r="A3" s="18">
+      <c r="A3" s="20">
         <v>106</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="36.85" spans="1:3">
-      <c r="A4" s="18">
+      <c r="A4" s="20">
         <v>107</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="18.45" spans="1:3">
-      <c r="A5" s="18">
+      <c r="A5" s="20">
         <v>108</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="18.45" spans="1:3">
-      <c r="A6" s="18">
+      <c r="A6" s="20">
         <v>109</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" ht="36.85" spans="1:3">
-      <c r="A7" s="18">
+      <c r="A7" s="20">
         <v>110</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19"/>
-    </row>
-    <row r="8" ht="18.45" spans="1:2">
-      <c r="A8" s="18">
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" ht="18.45" spans="1:3">
+      <c r="A8" s="20">
         <v>111</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" ht="55.3" spans="1:3">
-      <c r="A9" s="18">
+      <c r="C8" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" ht="92.15" spans="1:3">
+      <c r="A9" s="20">
         <v>112</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" ht="55.3" spans="1:3">
-      <c r="A10" s="18">
+      <c r="B9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" ht="129" spans="1:3">
+      <c r="A10" s="20">
         <v>113</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" ht="36.85" spans="1:3">
-      <c r="A11" s="18">
+      <c r="B10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" ht="147.45" spans="1:3">
+      <c r="A11" s="20">
         <v>114</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="22"/>
+      <c r="B11" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" ht="73.7" spans="1:3">
-      <c r="A12" s="18">
+      <c r="A12" s="20">
         <v>115</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" ht="147.45" spans="1:3">
-      <c r="A13" s="18">
+      <c r="B12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="129" spans="1:3">
+      <c r="A13" s="20">
         <v>116</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>21</v>
+      <c r="B13" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" ht="129" spans="1:3">
-      <c r="A14" s="18">
+      <c r="A14" s="20">
         <v>117</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>23</v>
+      <c r="B14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" ht="165.85" spans="1:3">
-      <c r="A15" s="18">
+      <c r="A15" s="20">
         <v>118</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="18">
+      <c r="B15" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="24"/>
+    </row>
+    <row r="16" ht="36.85" spans="1:3">
+      <c r="A16" s="20">
         <v>119</v>
       </c>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="18">
+      <c r="B16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="24"/>
+    </row>
+    <row r="17" ht="55.3" spans="1:3">
+      <c r="A17" s="20">
         <v>120</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="B17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="24"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="18">
+      <c r="A18" s="20">
         <v>121</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="18">
+      <c r="A19" s="20">
         <v>122</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="18">
+      <c r="A20" s="20">
         <v>123</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="18">
+      <c r="A21" s="20">
         <v>124</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="18">
+      <c r="A22" s="20">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="18">
+      <c r="A23" s="20">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="18">
+      <c r="A24" s="20">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="18">
+      <c r="A25" s="20">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="18">
+      <c r="A26" s="20">
         <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="18">
+      <c r="A27" s="20">
         <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="18">
+      <c r="A28" s="20">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="18">
+    <row r="29" spans="1:3">
+      <c r="A29" s="20">
         <v>132</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="18">
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="20">
         <v>133</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="18">
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="20">
         <v>134</v>
       </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="18">
+      <c r="A32" s="20">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="18">
+      <c r="A33" s="20">
         <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="18">
+      <c r="A34" s="20">
         <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="18">
+      <c r="A35" s="20">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="18">
+      <c r="A36" s="20">
         <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="18">
+      <c r="A37" s="20">
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="18">
+      <c r="A38" s="20">
         <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="18">
+      <c r="A39" s="20">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="18">
+      <c r="A40" s="20">
         <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="18">
+      <c r="A41" s="20">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="18">
+      <c r="A42" s="20">
         <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="18">
+      <c r="A43" s="20">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="18">
+      <c r="A44" s="20">
         <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="18">
+      <c r="A45" s="20">
         <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="18">
+      <c r="A46" s="20">
         <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="18">
+      <c r="A47" s="20">
         <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="18">
+      <c r="A48" s="20">
         <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="18">
+      <c r="A49" s="20">
         <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="18">
+      <c r="A50" s="20">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="18">
+      <c r="A51" s="20">
         <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="18">
+      <c r="A52" s="20">
         <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="18">
+      <c r="A53" s="20">
         <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="18">
+      <c r="A54" s="20">
         <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="18">
+      <c r="A55" s="20">
         <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="18">
+      <c r="A56" s="20">
         <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="18">
+      <c r="A57" s="20">
         <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="18">
+      <c r="A58" s="20">
         <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="18">
+      <c r="A59" s="20">
         <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="18">
+      <c r="A60" s="20">
         <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="18">
+      <c r="A61" s="20">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="18">
+      <c r="A62" s="20">
         <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="18">
+      <c r="A63" s="20">
         <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="18">
+      <c r="A64" s="20">
         <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="18">
+      <c r="A65" s="20">
         <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="18">
+      <c r="A66" s="20">
         <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="18">
+      <c r="A67" s="20">
         <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="18">
+      <c r="A68" s="20">
         <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="18">
+      <c r="A69" s="20">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="18">
+      <c r="A70" s="20">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="18">
+      <c r="A71" s="20">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="18">
+      <c r="A72" s="20">
         <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="18">
+      <c r="A73" s="20">
         <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="18">
+      <c r="A74" s="20">
         <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="18">
+      <c r="A75" s="20">
         <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="18">
+      <c r="A76" s="20">
         <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="18">
+      <c r="A77" s="20">
         <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="18">
+      <c r="A78" s="20">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="18">
+      <c r="A79" s="20">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="18">
+      <c r="A80" s="20">
         <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="18">
+      <c r="A81" s="20">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="18">
+      <c r="A82" s="20">
         <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="18">
+      <c r="A83" s="20">
         <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="18">
+      <c r="A84" s="20">
         <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="18">
+      <c r="A85" s="20">
         <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="18">
+      <c r="A86" s="20">
         <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="18">
+      <c r="A87" s="20">
         <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="18">
+      <c r="A88" s="20">
         <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="18">
+      <c r="A89" s="20">
         <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="18">
+      <c r="A90" s="20">
         <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="18">
+      <c r="A91" s="20">
         <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="18">
+      <c r="A92" s="20">
         <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="18">
+      <c r="A93" s="20">
         <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="18">
+      <c r="A94" s="20">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="18">
+      <c r="A95" s="20">
         <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="18">
+      <c r="A96" s="20">
         <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="18">
+      <c r="A97" s="20">
         <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="18">
+      <c r="A98" s="20">
         <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="18">
+      <c r="A99" s="20">
         <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="18">
+      <c r="A100" s="20">
         <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="18">
+      <c r="A101" s="20">
         <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="18">
+      <c r="A102" s="20">
         <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="18">
+      <c r="A103" s="20">
         <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="18">
+      <c r="A104" s="20">
         <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="18">
+      <c r="A105" s="20">
         <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="18">
+      <c r="A106" s="20">
         <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="18">
+      <c r="A107" s="20">
         <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="18">
+      <c r="A108" s="20">
         <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="18">
+      <c r="A109" s="20">
         <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="18">
+      <c r="A110" s="20">
         <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="18">
+      <c r="A111" s="20">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="18">
+      <c r="A112" s="20">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="18">
+      <c r="A113" s="20">
         <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="18">
+      <c r="A114" s="20">
         <v>217</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="18">
+      <c r="A115" s="20">
         <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="18">
+      <c r="A116" s="20">
         <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="18">
+      <c r="A117" s="20">
         <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="18">
+      <c r="A118" s="20">
         <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="18">
+      <c r="A119" s="20">
         <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="18">
+      <c r="A120" s="20">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="18">
+      <c r="A121" s="20">
         <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="18">
+      <c r="A122" s="20">
         <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="18">
+      <c r="A123" s="20">
         <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="18">
+      <c r="A124" s="20">
         <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="18">
+      <c r="A125" s="20">
         <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="18">
+      <c r="A126" s="20">
         <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="18">
+      <c r="A127" s="20">
         <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="18">
+      <c r="A128" s="20">
         <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="18">
+      <c r="A129" s="20">
         <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="18">
+      <c r="A130" s="20">
         <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="18">
+      <c r="A131" s="20">
         <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="18">
+      <c r="A132" s="20">
         <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="18">
+      <c r="A133" s="20">
         <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="18">
+      <c r="A134" s="20">
         <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="18">
+      <c r="A135" s="20">
         <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="18">
+      <c r="A136" s="20">
         <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="18">
+      <c r="A137" s="20">
         <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="18">
+      <c r="A138" s="20">
         <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="18">
+      <c r="A139" s="20">
         <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="18">
+      <c r="A140" s="20">
         <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="18">
+      <c r="A141" s="20">
         <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="18">
+      <c r="A142" s="20">
         <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="18">
+      <c r="A143" s="20">
         <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="18">
+      <c r="A144" s="20">
         <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="18">
+      <c r="A145" s="20">
         <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="18">
+      <c r="A146" s="20">
         <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="18">
+      <c r="A147" s="20">
         <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="18">
+      <c r="A148" s="20">
         <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="18">
+      <c r="A149" s="20">
         <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="18">
+      <c r="A150" s="20">
         <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="18">
+      <c r="A151" s="20">
         <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="18">
+      <c r="A152" s="20">
         <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="18">
+      <c r="A153" s="20">
         <v>256</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="18">
+      <c r="A154" s="20">
         <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="18">
+      <c r="A155" s="20">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="18">
+      <c r="A156" s="20">
         <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="18">
+      <c r="A157" s="20">
         <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="18">
+      <c r="A158" s="20">
         <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="18">
+      <c r="A159" s="20">
         <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="18">
+      <c r="A160" s="20">
         <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="18">
+      <c r="A161" s="20">
         <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="18">
+      <c r="A162" s="20">
         <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="18">
+      <c r="A163" s="20">
         <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="18">
+      <c r="A164" s="20">
         <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="18">
+      <c r="A165" s="20">
         <v>268</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="18">
+      <c r="A166" s="20">
         <v>269</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="18">
+      <c r="A167" s="20">
         <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="18">
+      <c r="A168" s="20">
         <v>271</v>
       </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="18">
+      <c r="A169" s="20">
         <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="18">
+      <c r="A170" s="20">
         <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="18">
+      <c r="A171" s="20">
         <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="18">
+      <c r="A172" s="20">
         <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="18">
+      <c r="A173" s="20">
         <v>276</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="18">
+      <c r="A174" s="20">
         <v>277</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="18">
+      <c r="A175" s="20">
         <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="18">
+      <c r="A176" s="20">
         <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="18">
+      <c r="A177" s="20">
         <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="18">
+      <c r="A178" s="20">
         <v>281</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="18">
+      <c r="A179" s="20">
         <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="18">
+      <c r="A180" s="20">
         <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="18">
+      <c r="A181" s="20">
         <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="18">
+      <c r="A182" s="20">
         <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="18">
+      <c r="A183" s="20">
         <v>286</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="18">
+      <c r="A184" s="20">
         <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="18">
+      <c r="A185" s="20">
         <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="18">
+      <c r="A186" s="20">
         <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="18">
+      <c r="A187" s="20">
         <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="18">
+      <c r="A188" s="20">
         <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="18">
+      <c r="A189" s="20">
         <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="18">
+      <c r="A190" s="20">
         <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="18">
+      <c r="A191" s="20">
         <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="18">
+      <c r="A192" s="20">
         <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="18">
+      <c r="A193" s="20">
         <v>296</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="18">
+      <c r="A194" s="20">
         <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="18">
+      <c r="A195" s="20">
         <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="18">
+      <c r="A196" s="20">
         <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="18">
+      <c r="A197" s="20">
         <v>300</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="18">
+      <c r="A198" s="20">
         <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="18">
+      <c r="A199" s="20">
         <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="18">
+      <c r="A200" s="20">
         <v>303</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="18">
+      <c r="A201" s="20">
         <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="18">
+      <c r="A202" s="20">
         <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="18">
+      <c r="A203" s="20">
         <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="18">
+      <c r="A204" s="20">
         <v>307</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="18">
+      <c r="A205" s="20">
         <v>308</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="18">
+      <c r="A206" s="20">
         <v>309</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="18">
+      <c r="A207" s="20">
         <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="18">
+      <c r="A208" s="20">
         <v>311</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="18">
+      <c r="A209" s="20">
         <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="18">
+      <c r="A210" s="20">
         <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="18">
+      <c r="A211" s="20">
         <v>314</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="18">
+      <c r="A212" s="20">
         <v>315</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="18">
+      <c r="A213" s="20">
         <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="18">
+      <c r="A214" s="20">
         <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="18">
+      <c r="A215" s="20">
         <v>318</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="18">
+      <c r="A216" s="20">
         <v>319</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="18">
+      <c r="A217" s="20">
         <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="18">
+      <c r="A218" s="20">
         <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" s="18">
+      <c r="A219" s="20">
         <v>322</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="18">
+      <c r="A220" s="20">
         <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" s="18">
+      <c r="A221" s="20">
         <v>324</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="18">
+      <c r="A222" s="20">
         <v>325</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" s="18">
+      <c r="A223" s="20">
         <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="18">
+      <c r="A224" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="18">
+      <c r="A225" s="20">
         <v>328</v>
       </c>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="18">
+      <c r="A226" s="20">
         <v>329</v>
       </c>
     </row>
     <row r="227" spans="1:1">
-      <c r="A227" s="18">
+      <c r="A227" s="20">
         <v>330</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="18">
+      <c r="A228" s="20">
         <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="18">
+      <c r="A229" s="20">
         <v>332</v>
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="18">
+      <c r="A230" s="20">
         <v>333</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="18">
+      <c r="A231" s="20">
         <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="18">
+      <c r="A232" s="20">
         <v>335</v>
       </c>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="18">
+      <c r="A233" s="20">
         <v>336</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="18">
+      <c r="A234" s="20">
         <v>337</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="18">
+      <c r="A235" s="20">
         <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="18">
+      <c r="A236" s="20">
         <v>339</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237" s="18">
+      <c r="A237" s="20">
         <v>340</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="18">
+      <c r="A238" s="20">
         <v>341</v>
       </c>
     </row>
     <row r="239" spans="1:1">
-      <c r="A239" s="18">
+      <c r="A239" s="20">
         <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="18">
+      <c r="A240" s="20">
         <v>343</v>
       </c>
     </row>
     <row r="241" spans="1:1">
-      <c r="A241" s="18">
+      <c r="A241" s="20">
         <v>344</v>
       </c>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="18">
+      <c r="A242" s="20">
         <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:1">
-      <c r="A243" s="18">
+      <c r="A243" s="20">
         <v>346</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="18">
+      <c r="A244" s="20">
         <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245" s="18">
+      <c r="A245" s="20">
         <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="18">
+      <c r="A246" s="20">
         <v>349</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" s="18">
+      <c r="A247" s="20">
         <v>350</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="18">
+      <c r="A248" s="20">
         <v>351</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" s="18">
+      <c r="A249" s="20">
         <v>352</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="18">
+      <c r="A250" s="20">
         <v>353</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" s="18">
+      <c r="A251" s="20">
         <v>354</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="18">
+      <c r="A252" s="20">
         <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:1">
-      <c r="A253" s="18">
+      <c r="A253" s="20">
         <v>356</v>
       </c>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="18">
+      <c r="A254" s="20">
         <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:1">
-      <c r="A255" s="18">
+      <c r="A255" s="20">
         <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="18">
+      <c r="A256" s="20">
         <v>359</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" s="18">
+      <c r="A257" s="20">
         <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="18">
+      <c r="A258" s="20">
         <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:1">
-      <c r="A259" s="18">
+      <c r="A259" s="20">
         <v>362</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="18">
+      <c r="A260" s="20">
         <v>363</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261" s="18">
+      <c r="A261" s="20">
         <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="18">
+      <c r="A262" s="20">
         <v>365</v>
       </c>
     </row>
@@ -3406,159 +3515,159 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:1">
       <c r="A17" s="12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="12" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="13" t="s">
-        <v>42</v>
+      <c r="A20" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" ht="15.45" spans="1:2">
-      <c r="A32" s="16" t="s">
-        <v>52</v>
+      <c r="A32" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="16" t="s">
-        <v>54</v>
+      <c r="A33" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3573,162 +3682,162 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="8.66019417475728" style="3"/>
-    <col min="2" max="2" width="33.2912621359223" style="13" customWidth="1"/>
-    <col min="3" max="3" width="78.1359223300971" style="13" customWidth="1"/>
+    <col min="2" max="2" width="33.2912621359223" style="15" customWidth="1"/>
+    <col min="3" max="3" width="78.1359223300971" style="15" customWidth="1"/>
     <col min="4" max="16384" width="8.66019417475728" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>62</v>
+      <c r="B2" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>64</v>
+      <c r="B3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>66</v>
+      <c r="B4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" s="4" customFormat="1" spans="1:3">
       <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>70</v>
+      <c r="C8" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>71</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="1" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>60</v>
+        <v>78</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>74</v>
+      <c r="B12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>75</v>
+      <c r="B13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="13" t="s">
-        <v>65</v>
+      <c r="B14" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:3">
       <c r="A16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="13" t="s">
-        <v>78</v>
+      <c r="B17" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" ht="77.15" spans="2:3">
-      <c r="B20" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>83</v>
+      <c r="B20" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" ht="46.3" spans="2:3">
-      <c r="B21" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>85</v>
+      <c r="B21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3740,52 +3849,46 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4"/>
   <cols>
+    <col min="1" max="1" width="10.6504854368932" customWidth="1"/>
+    <col min="2" max="2" width="12.3106796116505" customWidth="1"/>
+    <col min="5" max="5" width="31.0388349514563" customWidth="1"/>
     <col min="6" max="6" width="14.9708737864078" customWidth="1"/>
     <col min="7" max="7" width="13.3300970873786" customWidth="1"/>
     <col min="8" max="8" width="21.2912621359223" customWidth="1"/>
     <col min="10" max="10" width="34.1165048543689" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
-      <c r="B1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>88</v>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>92</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>44</v>
-      </c>
-      <c r="D2">
-        <v>32</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I2">
         <v>-100</v>
@@ -3793,29 +3896,41 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B3">
-        <f>11.5*B2</f>
-        <v>322</v>
+        <v>28</v>
       </c>
       <c r="C3">
-        <f>13*C2</f>
-        <v>572</v>
+        <v>44</v>
       </c>
       <c r="D3">
-        <v>572</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="I3">
         <v>-70</v>
       </c>
     </row>
-    <row r="4" spans="8:9">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4">
+        <f>11.5*B3</f>
+        <v>322</v>
+      </c>
+      <c r="C4">
+        <f>13*C3</f>
+        <v>572</v>
+      </c>
+      <c r="D4">
+        <v>572</v>
+      </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I4">
         <v>-50</v>
@@ -3823,7 +3938,7 @@
     </row>
     <row r="5" spans="8:9">
       <c r="H5" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="I5">
         <v>-20</v>
@@ -3831,40 +3946,120 @@
     </row>
     <row r="6" spans="8:10">
       <c r="H6" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I6">
         <v>-10</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" ht="14" customHeight="1" spans="8:10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="8:10">
       <c r="H7" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="8:9">
       <c r="H8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="8:9">
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="I9">
         <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" ht="30.85" spans="1:5">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3890,10 +4085,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3919,409 +4114,409 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="12" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:1">
       <c r="A6" s="12" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="12" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="12" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" spans="1:1">
       <c r="A10" s="9" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="12" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="12" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="12" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" s="10" customFormat="1" spans="1:1">
       <c r="A15" s="10" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" s="11" customFormat="1" spans="1:1">
       <c r="A16" s="11" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" s="11" customFormat="1" spans="1:1">
       <c r="A20" s="11" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" s="11" customFormat="1" spans="1:1">
       <c r="A24" s="11" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" s="11" customFormat="1" spans="1:1">
       <c r="A28" s="11" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:1">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:1">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:1">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" s="11" customFormat="1" spans="1:1">
       <c r="A36" s="11" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:1">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" ht="14" customHeight="1"/>
     <row r="41" s="10" customFormat="1" spans="1:1">
       <c r="A41" s="10" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" s="11" customFormat="1" spans="1:1">
       <c r="A42" s="11" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:1">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:1">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:1">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" s="11" customFormat="1" spans="1:1">
       <c r="A46" s="11" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:1">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" s="11" customFormat="1" spans="1:1">
       <c r="A48" s="11" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:1">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" s="11" customFormat="1" spans="1:1">
       <c r="A50" s="11" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1"/>
     <row r="53" s="10" customFormat="1" spans="1:1">
       <c r="A53" s="10" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" s="11" customFormat="1" spans="1:1">
       <c r="A54" s="11" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" s="11" customFormat="1" spans="1:1">
       <c r="A58" s="11" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" s="11" customFormat="1" spans="1:1">
       <c r="A60" s="11" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" s="11" customFormat="1" spans="1:1">
       <c r="A62" s="11" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" s="11" customFormat="1" spans="1:1">
       <c r="A64" s="11" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" s="10" customFormat="1" spans="1:1">
       <c r="A67" s="10" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" s="11" customFormat="1" spans="1:1">
       <c r="A68" s="11" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" s="11" customFormat="1" spans="1:1">
       <c r="A70" s="11" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" s="11" customFormat="1" spans="1:1">
       <c r="A73" s="11" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" s="11" customFormat="1" spans="1:1">
       <c r="A75" s="11" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" s="11" customFormat="1" spans="1:1">
       <c r="A77" s="11" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" s="10" customFormat="1" spans="1:1">
       <c r="A80" s="10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" s="11" customFormat="1" spans="1:1">
       <c r="A81" s="11" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" s="11" customFormat="1" spans="1:1">
       <c r="A83" s="11" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" s="11" customFormat="1" spans="1:1">
       <c r="A85" s="11" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="87" s="11" customFormat="1" spans="1:1">
       <c r="A87" s="11" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4349,10 +4544,10 @@
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
@@ -4360,7 +4555,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
@@ -4368,10 +4563,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -4379,10 +4574,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:2">
@@ -4390,24 +4585,24 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
       <c r="A6" s="3"/>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4415,7 +4610,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4423,7 +4618,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4431,10 +4626,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4442,10 +4637,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4453,7 +4648,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4461,10 +4656,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4472,7 +4667,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4480,7 +4675,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4488,10 +4683,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4499,18 +4694,18 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4518,10 +4713,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4529,10 +4724,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4540,10 +4735,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4551,10 +4746,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C23" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4562,10 +4757,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4573,18 +4768,18 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4592,10 +4787,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="C28" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4603,7 +4798,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4611,10 +4806,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4622,10 +4817,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C31" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4633,7 +4828,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4641,10 +4836,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C33" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4652,10 +4847,10 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="C34" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4663,10 +4858,10 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="C35" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4674,10 +4869,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C36" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4685,21 +4880,21 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="C37" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -4707,10 +4902,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="C40" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -4718,10 +4913,10 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -4729,10 +4924,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -4740,10 +4935,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="C43" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4751,73 +4946,73 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="B45" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="C45" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="7" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C46" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="7" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="B47" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="7" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="B48" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="7" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B49" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="C49" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="7" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="B50" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="C50" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4825,10 +5020,10 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="C51" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4836,10 +5031,10 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C52" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day121 - 2026-01-04 23:21:13
</commit_message>
<xml_diff>
--- a/Devlog每日紀錄.xlsx
+++ b/Devlog每日紀錄.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21882" windowHeight="11057" tabRatio="621" activeTab="3"/>
+    <workbookView windowWidth="21882" windowHeight="11057" tabRatio="621"/>
   </bookViews>
   <sheets>
     <sheet name="Devlog日誌" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283">
   <si>
     <t>Devlog</t>
   </si>
@@ -122,13 +122,36 @@
 水平衝刺位移問題修正(SkillDashing順序問題，被StopCoroutine關掉了)</t>
   </si>
   <si>
-    <t>程式：
-通關後結算畫面
+    <r>
+      <t xml:space="preserve">程式：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <charset val="134"/>
+      </rPr>
+      <t>通關後結算畫面
+打怪後升級加能力，可以實質變強，設計不同關卡難度，測試一關接一關的玩法</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF1D41D5"/>
+        <rFont val="微軟正黑體"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 掉落物系統
 背包系統
 腳色受傷動畫繪製
 腳色死亡動畫重製
 關卡失敗條件設定</t>
+    </r>
   </si>
   <si>
     <t>繪製草坪、草群
@@ -140,10 +163,35 @@
 底部Move Collider已可不互相碰撞</t>
   </si>
   <si>
-    <t>美術：
-城防結界核心
+    <r>
+      <t xml:space="preserve">美術：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <charset val="134"/>
+      </rPr>
+      <t>城防結界核心
+MOBA操控玩法
+四個技能(冷卻、傷害設計)
+主角、Q劍氣、W下斬、E上斬、R奧義次元斬不被斷招有背影</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF1D41D5"/>
+        <rFont val="微軟正黑體"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 前景灌木叢、中景土地、灌木叢中景樹木、遠景樹林、山脈繪製
 先看概念設計、場景規劃</t>
+    </r>
   </si>
   <si>
     <t>草地雜訊、泥土雜訊、邊界密度、行動空間留白、邊界草20-30%布置完成
@@ -160,9 +208,15 @@
 通關後等待一下才允許點擊返回，完成</t>
   </si>
   <si>
-    <t xml:space="preserve">四個敵人依照32PPU，飽和度30上下，重繪
+    <t>四個敵人依照32PPU，飽和度30上下，重繪
 Sprite pivot底部客製高度完成
-</t>
+非Q版主角Idle腳色及動畫試繪完成(不在優化、保持原Q版)，先將遊戲循環內容完成，在優化各種細節</t>
+  </si>
+  <si>
+    <t>完成Enemy005
+腳色重新綁定為只控制一隻，並且使用QWER
+重新建立腳色結構，已修正敵人血條翻轉，高度跟隨Sprite
+實作兩個實用Player、EnemyScreenDebug，可以即時顯示StateComponent的狀態</t>
   </si>
   <si>
     <t>訓練法一：世界拆解練習（每天 15–30 分）</t>
@@ -954,7 +1008,7 @@
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,6 +1222,13 @@
       <sz val="11"/>
       <color rgb="FF1D41D5"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="微軟正黑體"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2065,8 +2126,8 @@
   <sheetPr/>
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.4" outlineLevelCol="2"/>
@@ -2207,7 +2268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="129" spans="1:3">
+    <row r="13" ht="147.45" spans="1:3">
       <c r="A13" s="20">
         <v>116</v>
       </c>
@@ -2247,7 +2308,7 @@
       </c>
       <c r="C16" s="24"/>
     </row>
-    <row r="17" ht="55.3" spans="1:3">
+    <row r="17" ht="73.7" spans="1:3">
       <c r="A17" s="20">
         <v>120</v>
       </c>
@@ -2256,9 +2317,12 @@
       </c>
       <c r="C17" s="24"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" ht="92.15" spans="1:3">
       <c r="A18" s="20">
         <v>121</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="24"/>
     </row>
@@ -3515,159 +3579,159 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:1">
       <c r="A17" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" ht="15.45" spans="1:2">
       <c r="A32" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3695,149 +3759,149 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" s="4" customFormat="1" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="1" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:3">
       <c r="A16" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" ht="77.15" spans="2:3">
       <c r="B20" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" ht="46.3" spans="2:3">
       <c r="B21" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3851,8 +3915,8 @@
   <sheetPr/>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66019417475728" defaultRowHeight="15.4"/>
@@ -3868,27 +3932,27 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2">
         <v>-100</v>
@@ -3896,7 +3960,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>28</v>
@@ -3908,7 +3972,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I3">
         <v>-70</v>
@@ -3916,7 +3980,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <f>11.5*B3</f>
@@ -3930,7 +3994,7 @@
         <v>572</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I4">
         <v>-50</v>
@@ -3938,7 +4002,7 @@
     </row>
     <row r="5" spans="8:9">
       <c r="H5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I5">
         <v>-20</v>
@@ -3946,29 +4010,29 @@
     </row>
     <row r="6" spans="8:10">
       <c r="H6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I6">
         <v>-10</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="8:10">
       <c r="H7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="8:9">
       <c r="H8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -3976,19 +4040,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I9">
         <v>50</v>
@@ -3996,67 +4060,67 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B10">
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" ht="30.85" spans="1:5">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B19">
         <v>35</v>
@@ -4085,10 +4149,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4114,409 +4178,409 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:1">
       <c r="A6" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" spans="1:1">
       <c r="A10" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" s="10" customFormat="1" spans="1:1">
       <c r="A15" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" s="11" customFormat="1" spans="1:1">
       <c r="A16" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" s="11" customFormat="1" spans="1:1">
       <c r="A20" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" s="11" customFormat="1" spans="1:1">
       <c r="A24" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" s="11" customFormat="1" spans="1:1">
       <c r="A28" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:1">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:1">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:1">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" s="11" customFormat="1" spans="1:1">
       <c r="A36" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:1">
       <c r="A37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" ht="14" customHeight="1"/>
     <row r="41" s="10" customFormat="1" spans="1:1">
       <c r="A41" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" s="11" customFormat="1" spans="1:1">
       <c r="A42" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:1">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:1">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:1">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" s="11" customFormat="1" spans="1:1">
       <c r="A46" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:1">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" s="11" customFormat="1" spans="1:1">
       <c r="A48" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:1">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" s="11" customFormat="1" spans="1:1">
       <c r="A50" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1"/>
     <row r="53" s="10" customFormat="1" spans="1:1">
       <c r="A53" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" s="11" customFormat="1" spans="1:1">
       <c r="A54" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" s="11" customFormat="1" spans="1:1">
       <c r="A58" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" s="11" customFormat="1" spans="1:1">
       <c r="A60" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" s="11" customFormat="1" spans="1:1">
       <c r="A62" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" s="11" customFormat="1" spans="1:1">
       <c r="A64" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" s="10" customFormat="1" spans="1:1">
       <c r="A67" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" s="11" customFormat="1" spans="1:1">
       <c r="A68" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" s="11" customFormat="1" spans="1:1">
       <c r="A70" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" s="11" customFormat="1" spans="1:1">
       <c r="A73" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" s="11" customFormat="1" spans="1:1">
       <c r="A75" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" s="11" customFormat="1" spans="1:1">
       <c r="A77" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" s="10" customFormat="1" spans="1:1">
       <c r="A80" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" s="11" customFormat="1" spans="1:1">
       <c r="A81" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" s="11" customFormat="1" spans="1:1">
       <c r="A83" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" s="11" customFormat="1" spans="1:1">
       <c r="A85" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" s="11" customFormat="1" spans="1:1">
       <c r="A87" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4544,10 +4608,10 @@
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
@@ -4555,7 +4619,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
@@ -4563,10 +4627,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:3">
@@ -4574,10 +4638,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:2">
@@ -4585,24 +4649,24 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:3">
       <c r="A6" s="3"/>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4610,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4618,7 +4682,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4626,10 +4690,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4637,10 +4701,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4648,7 +4712,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4656,10 +4720,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4667,7 +4731,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4675,7 +4739,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="15.45" spans="1:3">
@@ -4683,10 +4747,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="15.45" spans="1:2">
@@ -4694,18 +4758,18 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4713,10 +4777,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4724,10 +4788,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4735,10 +4799,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4746,10 +4810,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4757,10 +4821,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4768,18 +4832,18 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4787,10 +4851,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4798,7 +4862,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4806,10 +4870,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4817,10 +4881,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C31" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4828,7 +4892,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4836,10 +4900,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C33" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4847,10 +4911,10 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4858,10 +4922,10 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C35" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4869,10 +4933,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4880,21 +4944,21 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C37" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -4902,10 +4966,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C40" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -4913,10 +4977,10 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C41" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -4924,10 +4988,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C42" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -4935,10 +4999,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C43" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4946,73 +5010,73 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C46" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C47" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B48" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C48" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B49" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C49" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B50" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C50" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -5020,10 +5084,10 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C51" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5031,10 +5095,10 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C52" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>